<commit_message>
Ajout des fonctions avec les param.
</commit_message>
<xml_diff>
--- a/ExerciceExcel3/Islam_Shafaatul_Excel_Exercice03_FonctionsMathematiques.xlsx
+++ b/ExerciceExcel3/Islam_Shafaatul_Excel_Exercice03_FonctionsMathematiques.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CVM\Outil de gestion\GitHub2022\ExerciceExcel3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fc197a25ccdc5fa/Desktop/GitHub2022/ExerciceExcel3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F94E178-8919-4BF0-8E90-5D9E5E3834FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{1F94E178-8919-4BF0-8E90-5D9E5E3834FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB47678A-72E7-44DC-AB4E-A15268CC2DAF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonctions mathématiques" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
   <si>
     <t>Objectifs de cet exercice</t>
   </si>
@@ -1330,6 +1330,42 @@
       <t>d</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">y = a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>∙</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> | b ∙  x + c | + d</t>
+    </r>
+  </si>
+  <si>
+    <t>y = a ∙ x + b</t>
+  </si>
+  <si>
+    <t>y = a ∙ x</t>
+  </si>
+  <si>
+    <t>y = a ∙ ln( b ∙ x + c ) + d</t>
+  </si>
+  <si>
+    <t>y = a ∙ b</t>
+  </si>
 </sst>
 </file>
 
@@ -1339,7 +1375,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1666,6 +1702,35 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2935,7 +3000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="245">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
@@ -3701,6 +3766,44 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="57" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="57" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="37" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="38" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="45" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="46" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="49" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="50" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -3777,29 +3880,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="37" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="38" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="45" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="46" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="49" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="50" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="56" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="53" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3821,24 +3909,28 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="43" fillId="56" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="47" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="45" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="56" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="57" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="57" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="57" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3875,7 +3967,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7869,7 +7961,7 @@
             <a:pPr>
               <a:defRPr sz="800"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="143401640"/>
@@ -7895,7 +7987,7 @@
             <a:pPr>
               <a:defRPr sz="800"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="143401248"/>
@@ -7913,7 +8005,7 @@
           <a:pPr>
             <a:defRPr sz="600"/>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7939,7 +8031,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="fr-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -9968,7 +10060,7 @@
             <a:pPr>
               <a:defRPr sz="800"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="142439888"/>
@@ -9996,7 +10088,7 @@
             <a:pPr>
               <a:defRPr sz="800"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="143403992"/>
@@ -10016,7 +10108,7 @@
           <a:pPr>
             <a:defRPr sz="600"/>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -10450,92 +10542,92 @@
       <selection activeCell="G21" sqref="G21:H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="0.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="1.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="0.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="4" customWidth="1"/>
-    <col min="7" max="10" width="8.28515625" style="5" customWidth="1"/>
-    <col min="11" max="12" width="8.28515625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="3.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="0.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="0.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="9.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="0.5703125" style="33" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="0.5703125" style="33" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="0.5703125" style="33" customWidth="1"/>
-    <col min="24" max="24" width="9.42578125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="0.5703125" style="33" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="0.5703125" style="33" customWidth="1"/>
-    <col min="28" max="28" width="9.42578125" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="1.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="1.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="0.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.7265625" style="4" customWidth="1"/>
+    <col min="7" max="10" width="8.26953125" style="5" customWidth="1"/>
+    <col min="11" max="12" width="8.26953125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="5.54296875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="3.26953125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="0.54296875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="9.453125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="0.7265625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="0.54296875" style="33" customWidth="1"/>
+    <col min="20" max="20" width="9.453125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="0.54296875" style="33" customWidth="1"/>
+    <col min="22" max="22" width="9.453125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="0.54296875" style="33" customWidth="1"/>
+    <col min="24" max="24" width="9.453125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="0.54296875" style="33" customWidth="1"/>
+    <col min="26" max="26" width="9.453125" style="2" customWidth="1"/>
+    <col min="27" max="27" width="0.54296875" style="33" customWidth="1"/>
+    <col min="28" max="28" width="9.453125" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:29" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="201" t="s">
+    <row r="1" spans="2:29" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="213" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="201"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="201"/>
-      <c r="I2" s="201"/>
-      <c r="J2" s="201"/>
-      <c r="K2" s="201"/>
-      <c r="L2" s="201"/>
-      <c r="M2" s="201"/>
-      <c r="N2" s="201"/>
-      <c r="O2" s="201"/>
-      <c r="P2" s="201"/>
-      <c r="Q2" s="201"/>
-      <c r="R2" s="201"/>
-      <c r="S2" s="201"/>
-      <c r="T2" s="201"/>
-      <c r="U2" s="201"/>
-      <c r="V2" s="201"/>
-      <c r="W2" s="201"/>
-      <c r="X2" s="201"/>
-      <c r="Y2" s="201"/>
-      <c r="Z2" s="201"/>
-      <c r="AA2" s="201"/>
-      <c r="AB2" s="201"/>
-    </row>
-    <row r="3" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
+      <c r="H2" s="213"/>
+      <c r="I2" s="213"/>
+      <c r="J2" s="213"/>
+      <c r="K2" s="213"/>
+      <c r="L2" s="213"/>
+      <c r="M2" s="213"/>
+      <c r="N2" s="213"/>
+      <c r="O2" s="213"/>
+      <c r="P2" s="213"/>
+      <c r="Q2" s="213"/>
+      <c r="R2" s="213"/>
+      <c r="S2" s="213"/>
+      <c r="T2" s="213"/>
+      <c r="U2" s="213"/>
+      <c r="V2" s="213"/>
+      <c r="W2" s="213"/>
+      <c r="X2" s="213"/>
+      <c r="Y2" s="213"/>
+      <c r="Z2" s="213"/>
+      <c r="AA2" s="213"/>
+      <c r="AB2" s="213"/>
+    </row>
+    <row r="3" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="29"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="202" t="s">
+      <c r="E4" s="214" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="202"/>
-      <c r="G4" s="204" t="s">
+      <c r="F4" s="214"/>
+      <c r="G4" s="216" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="205"/>
-      <c r="I4" s="205"/>
-      <c r="J4" s="205"/>
-      <c r="K4" s="205"/>
-      <c r="L4" s="205"/>
+      <c r="H4" s="217"/>
+      <c r="I4" s="217"/>
+      <c r="J4" s="217"/>
+      <c r="K4" s="217"/>
+      <c r="L4" s="217"/>
       <c r="M4" s="21"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
     </row>
-    <row r="5" spans="2:29" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:29" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="30"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="203"/>
-      <c r="F5" s="203"/>
+      <c r="E5" s="215"/>
+      <c r="F5" s="215"/>
       <c r="G5" s="17" t="s">
         <v>16</v>
       </c>
@@ -10558,7 +10650,7 @@
       <c r="P5" s="16"/>
       <c r="Q5" s="16"/>
     </row>
-    <row r="6" spans="2:29" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:29" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
@@ -10571,12 +10663,12 @@
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
     </row>
-    <row r="7" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C7" s="87"/>
-      <c r="D7" s="213" t="s">
+      <c r="D7" s="225" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="213"/>
+      <c r="E7" s="225"/>
       <c r="F7" s="178" t="s">
         <v>41</v>
       </c>
@@ -10594,10 +10686,10 @@
       </c>
       <c r="K7" s="160"/>
       <c r="L7" s="161"/>
-      <c r="M7" s="211"/>
-      <c r="N7" s="211"/>
-      <c r="O7" s="211"/>
-      <c r="P7" s="211"/>
+      <c r="M7" s="223"/>
+      <c r="N7" s="223"/>
+      <c r="O7" s="223"/>
+      <c r="P7" s="223"/>
       <c r="Q7" s="88"/>
       <c r="R7" s="89"/>
       <c r="S7" s="34"/>
@@ -10606,7 +10698,7 @@
       <c r="Y7" s="34"/>
       <c r="AA7" s="34"/>
     </row>
-    <row r="8" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="22"/>
       <c r="D8" s="12"/>
       <c r="E8" s="22"/>
@@ -10629,12 +10721,12 @@
       <c r="Y8" s="34"/>
       <c r="AA8" s="34"/>
     </row>
-    <row r="9" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="98"/>
-      <c r="D9" s="214" t="s">
+      <c r="D9" s="226" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="214"/>
+      <c r="E9" s="226"/>
       <c r="F9" s="180" t="s">
         <v>42</v>
       </c>
@@ -10648,10 +10740,10 @@
       <c r="J9" s="165"/>
       <c r="K9" s="165"/>
       <c r="L9" s="165"/>
-      <c r="M9" s="212"/>
-      <c r="N9" s="212"/>
-      <c r="O9" s="212"/>
-      <c r="P9" s="212"/>
+      <c r="M9" s="224"/>
+      <c r="N9" s="224"/>
+      <c r="O9" s="224"/>
+      <c r="P9" s="224"/>
       <c r="Q9" s="99"/>
       <c r="R9" s="90"/>
       <c r="S9" s="100"/>
@@ -10666,7 +10758,7 @@
       <c r="AB9" s="39"/>
       <c r="AC9" s="22"/>
     </row>
-    <row r="10" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="22"/>
       <c r="D10" s="12"/>
       <c r="E10" s="22"/>
@@ -10695,12 +10787,12 @@
       <c r="AB10" s="39"/>
       <c r="AC10" s="22"/>
     </row>
-    <row r="11" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="110"/>
-      <c r="D11" s="215" t="s">
+      <c r="D11" s="227" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="215"/>
+      <c r="E11" s="227"/>
       <c r="F11" s="181" t="s">
         <v>43</v>
       </c>
@@ -10716,10 +10808,10 @@
       <c r="J11" s="168"/>
       <c r="K11" s="168"/>
       <c r="L11" s="168"/>
-      <c r="M11" s="218"/>
-      <c r="N11" s="218"/>
-      <c r="O11" s="218"/>
-      <c r="P11" s="218"/>
+      <c r="M11" s="205"/>
+      <c r="N11" s="205"/>
+      <c r="O11" s="205"/>
+      <c r="P11" s="205"/>
       <c r="Q11" s="111"/>
       <c r="R11" s="91"/>
       <c r="S11" s="112"/>
@@ -10734,7 +10826,7 @@
       <c r="AB11" s="35"/>
       <c r="AC11" s="22"/>
     </row>
-    <row r="12" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="22"/>
       <c r="D12" s="12"/>
       <c r="E12" s="22"/>
@@ -10763,12 +10855,12 @@
       <c r="AB12" s="35"/>
       <c r="AC12" s="22"/>
     </row>
-    <row r="13" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="122"/>
-      <c r="D13" s="216" t="s">
+      <c r="D13" s="228" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="216"/>
+      <c r="E13" s="228"/>
       <c r="F13" s="182" t="s">
         <v>44</v>
       </c>
@@ -10786,10 +10878,10 @@
       </c>
       <c r="K13" s="171"/>
       <c r="L13" s="171"/>
-      <c r="M13" s="217"/>
-      <c r="N13" s="217"/>
-      <c r="O13" s="217"/>
-      <c r="P13" s="217"/>
+      <c r="M13" s="204"/>
+      <c r="N13" s="204"/>
+      <c r="O13" s="204"/>
+      <c r="P13" s="204"/>
       <c r="Q13" s="123"/>
       <c r="R13" s="93"/>
       <c r="S13" s="124"/>
@@ -10804,7 +10896,7 @@
       <c r="AB13" s="36"/>
       <c r="AC13" s="22"/>
     </row>
-    <row r="14" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="22"/>
       <c r="D14" s="12"/>
       <c r="E14" s="22"/>
@@ -10833,12 +10925,12 @@
       <c r="AB14" s="36"/>
       <c r="AC14" s="22"/>
     </row>
-    <row r="15" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="133"/>
-      <c r="D15" s="220" t="s">
+      <c r="D15" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="220"/>
+      <c r="E15" s="207"/>
       <c r="F15" s="183" t="s">
         <v>45</v>
       </c>
@@ -10858,10 +10950,10 @@
         <v>-20</v>
       </c>
       <c r="L15" s="174"/>
-      <c r="M15" s="219"/>
-      <c r="N15" s="219"/>
-      <c r="O15" s="219"/>
-      <c r="P15" s="219"/>
+      <c r="M15" s="206"/>
+      <c r="N15" s="206"/>
+      <c r="O15" s="206"/>
+      <c r="P15" s="206"/>
       <c r="Q15" s="135"/>
       <c r="R15" s="94"/>
       <c r="S15" s="136"/>
@@ -10876,7 +10968,7 @@
       <c r="AB15" s="38"/>
       <c r="AC15" s="22"/>
     </row>
-    <row r="16" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:29" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="22"/>
       <c r="D16" s="12"/>
       <c r="E16" s="22"/>
@@ -10905,12 +10997,12 @@
       <c r="AB16" s="38"/>
       <c r="AC16" s="22"/>
     </row>
-    <row r="17" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="143"/>
-      <c r="D17" s="222" t="s">
+      <c r="D17" s="209" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="222"/>
+      <c r="E17" s="209"/>
       <c r="F17" s="184" t="s">
         <v>46</v>
       </c>
@@ -10928,10 +11020,10 @@
       </c>
       <c r="K17" s="177"/>
       <c r="L17" s="177"/>
-      <c r="M17" s="221"/>
-      <c r="N17" s="221"/>
-      <c r="O17" s="221"/>
-      <c r="P17" s="221"/>
+      <c r="M17" s="208"/>
+      <c r="N17" s="208"/>
+      <c r="O17" s="208"/>
+      <c r="P17" s="208"/>
       <c r="Q17" s="145"/>
       <c r="R17" s="90"/>
       <c r="S17" s="144"/>
@@ -10946,7 +11038,7 @@
       <c r="AB17" s="146"/>
       <c r="AC17" s="22"/>
     </row>
-    <row r="18" spans="2:29" ht="3" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:29" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M18" s="33"/>
       <c r="Q18" s="33"/>
       <c r="R18" s="95"/>
@@ -10956,7 +11048,7 @@
       <c r="Z18" s="140"/>
       <c r="AB18" s="147"/>
     </row>
-    <row r="19" spans="2:29" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:29" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M19" s="33"/>
       <c r="Q19" s="33"/>
       <c r="R19" s="95"/>
@@ -10966,26 +11058,26 @@
       <c r="Z19" s="140"/>
       <c r="AB19" s="147"/>
     </row>
-    <row r="20" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
-      <c r="E20" s="202" t="s">
+      <c r="E20" s="214" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="206"/>
-      <c r="G20" s="209" t="s">
+      <c r="F20" s="218"/>
+      <c r="G20" s="221" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="198"/>
-      <c r="I20" s="198" t="s">
+      <c r="H20" s="210"/>
+      <c r="I20" s="210" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="198"/>
-      <c r="K20" s="198" t="s">
+      <c r="J20" s="210"/>
+      <c r="K20" s="210" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="199"/>
+      <c r="L20" s="211"/>
       <c r="M20" s="44"/>
       <c r="N20" s="45"/>
       <c r="O20" s="45"/>
@@ -10998,25 +11090,25 @@
       <c r="Z20" s="140"/>
       <c r="AB20" s="147"/>
     </row>
-    <row r="21" spans="2:29" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:29" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
-      <c r="E21" s="207"/>
-      <c r="F21" s="208"/>
-      <c r="G21" s="210">
+      <c r="E21" s="219"/>
+      <c r="F21" s="220"/>
+      <c r="G21" s="222">
         <v>-10</v>
       </c>
-      <c r="H21" s="210"/>
-      <c r="I21" s="210">
+      <c r="H21" s="222"/>
+      <c r="I21" s="222">
         <v>0.2</v>
       </c>
-      <c r="J21" s="210"/>
-      <c r="K21" s="200">
+      <c r="J21" s="222"/>
+      <c r="K21" s="212">
         <f>G21+100*I21</f>
         <v>10</v>
       </c>
-      <c r="L21" s="200"/>
+      <c r="L21" s="212"/>
       <c r="M21" s="47"/>
       <c r="N21" s="48"/>
       <c r="O21" s="48"/>
@@ -11029,7 +11121,7 @@
       <c r="Z21" s="140"/>
       <c r="AB21" s="147"/>
     </row>
-    <row r="22" spans="2:29" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:29" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P22" s="50"/>
       <c r="Q22" s="33"/>
       <c r="R22" s="95"/>
@@ -11039,7 +11131,7 @@
       <c r="Z22" s="140"/>
       <c r="AB22" s="147"/>
     </row>
-    <row r="23" spans="2:29" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:29" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P23" s="50"/>
       <c r="Q23" s="33"/>
       <c r="R23" s="95"/>
@@ -11049,7 +11141,7 @@
       <c r="Z23" s="140"/>
       <c r="AB23" s="147"/>
     </row>
-    <row r="24" spans="2:29" s="7" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:29" s="7" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -11089,7 +11181,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
       <c r="N25" s="53">
         <v>1</v>
@@ -11130,7 +11222,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N26" s="53">
         <v>2</v>
       </c>
@@ -11170,7 +11262,7 @@
         <v>48.176784432060458</v>
       </c>
     </row>
-    <row r="27" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N27" s="53">
         <v>3</v>
       </c>
@@ -11210,7 +11302,7 @@
         <v>46.635277633787879</v>
       </c>
     </row>
-    <row r="28" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -11258,7 +11350,7 @@
         <v>45.299963707542659</v>
       </c>
     </row>
-    <row r="29" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -11306,7 +11398,7 @@
         <v>44.122133350978828</v>
       </c>
     </row>
-    <row r="30" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -11354,7 +11446,7 @@
         <v>43.068528194400564</v>
       </c>
     </row>
-    <row r="31" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -11402,7 +11494,7 @@
         <v>42.115426396357314</v>
       </c>
     </row>
-    <row r="32" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -11450,7 +11542,7 @@
         <v>41.245312626461022</v>
       </c>
     </row>
-    <row r="33" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -11498,7 +11590,7 @@
         <v>40.444885549725655</v>
       </c>
     </row>
-    <row r="34" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -11546,7 +11638,7 @@
         <v>39.703805828188443</v>
       </c>
     </row>
-    <row r="35" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -11594,7 +11686,7 @@
         <v>39.013877113318927</v>
       </c>
     </row>
-    <row r="36" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -11642,7 +11734,7 @@
         <v>38.368491901943216</v>
       </c>
     </row>
-    <row r="37" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -11690,7 +11782,7 @@
         <v>37.762245683778865</v>
       </c>
     </row>
-    <row r="38" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -11738,7 +11830,7 @@
         <v>37.190661545379378</v>
       </c>
     </row>
-    <row r="39" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -11786,7 +11878,7 @@
         <v>36.649989332676611</v>
       </c>
     </row>
-    <row r="40" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -11834,7 +11926,7 @@
         <v>36.137056388801113</v>
       </c>
     </row>
-    <row r="41" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -11882,7 +11974,7 @@
         <v>35.649154747106792</v>
       </c>
     </row>
-    <row r="42" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -11930,7 +12022,7 @@
         <v>35.183954590757857</v>
       </c>
     </row>
-    <row r="43" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -11978,7 +12070,7 @@
         <v>34.739436965049521</v>
       </c>
     </row>
-    <row r="44" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -12026,7 +12118,7 @@
         <v>34.313840820861557</v>
       </c>
     </row>
-    <row r="45" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -12074,7 +12166,7 @@
         <v>33.905620875659011</v>
       </c>
     </row>
-    <row r="46" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -12122,7 +12214,7 @@
         <v>33.513413744126197</v>
       </c>
     </row>
-    <row r="47" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -12170,7 +12262,7 @@
         <v>33.136010464297726</v>
       </c>
     </row>
-    <row r="48" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -12218,7 +12310,7 @@
         <v>32.772334022588979</v>
       </c>
     </row>
-    <row r="49" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -12266,7 +12358,7 @@
         <v>32.421420824476272</v>
       </c>
     </row>
-    <row r="50" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -12314,7 +12406,7 @@
         <v>32.082405307719455</v>
       </c>
     </row>
-    <row r="51" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -12362,7 +12454,7 @@
         <v>31.754507079489549</v>
       </c>
     </row>
-    <row r="52" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -12410,7 +12502,7 @@
         <v>31.437020096343744</v>
       </c>
     </row>
-    <row r="53" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -12458,7 +12550,7 @@
         <v>31.129303509676205</v>
       </c>
     </row>
-    <row r="54" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -12506,7 +12598,7 @@
         <v>30.830773878179397</v>
       </c>
     </row>
-    <row r="55" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -12554,7 +12646,7 @@
         <v>30.540898509446873</v>
       </c>
     </row>
-    <row r="56" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -12602,7 +12694,7 @@
         <v>30.259189739779909</v>
       </c>
     </row>
-    <row r="57" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -12650,7 +12742,7 @@
         <v>29.985199997898761</v>
       </c>
     </row>
-    <row r="58" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -12698,7 +12790,7 @@
         <v>29.718517527077147</v>
       </c>
     </row>
-    <row r="59" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -12746,7 +12838,7 @@
         <v>29.458762663044542</v>
       </c>
     </row>
-    <row r="60" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -12794,7 +12886,7 @@
         <v>29.205584583201642</v>
       </c>
     </row>
-    <row r="61" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -12842,7 +12934,7 @@
         <v>28.958658457297929</v>
       </c>
     </row>
-    <row r="62" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -12890,7 +12982,7 @@
         <v>28.71768294150732</v>
       </c>
     </row>
-    <row r="63" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -12938,7 +13030,7 @@
         <v>28.48237796740538</v>
       </c>
     </row>
-    <row r="64" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -12986,7 +13078,7 @@
         <v>28.252482785158396</v>
       </c>
     </row>
-    <row r="65" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -13034,7 +13126,7 @@
         <v>28.027754226637811</v>
       </c>
     </row>
-    <row r="66" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -13082,7 +13174,7 @@
         <v>27.807965159450056</v>
       </c>
     </row>
-    <row r="67" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -13130,7 +13222,7 @@
         <v>27.592903107240421</v>
       </c>
     </row>
-    <row r="68" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -13178,7 +13270,7 @@
         <v>27.3823690152621</v>
       </c>
     </row>
-    <row r="69" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -13226,7 +13318,7 @@
         <v>27.176176143234741</v>
       </c>
     </row>
-    <row r="70" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -13274,7 +13366,7 @@
         <v>26.974149070059546</v>
       </c>
     </row>
-    <row r="71" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -13322,7 +13414,7 @@
         <v>26.776122797097749</v>
       </c>
     </row>
-    <row r="72" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -13370,7 +13462,7 @@
         <v>26.581941938526729</v>
       </c>
     </row>
-    <row r="73" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N73" s="53">
         <v>49</v>
       </c>
@@ -13408,7 +13500,7 @@
         <v>26.391459988819786</v>
       </c>
     </row>
-    <row r="74" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N74" s="53">
         <v>50</v>
       </c>
@@ -13446,7 +13538,7 @@
         <v>26.204538658698265</v>
       </c>
     </row>
-    <row r="75" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N75" s="53">
         <v>51</v>
       </c>
@@ -13484,7 +13576,7 @@
         <v>26.021047272016297</v>
       </c>
     </row>
-    <row r="76" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N76" s="53">
         <v>52</v>
       </c>
@@ -13522,7 +13614,7 @@
         <v>25.840862216989514</v>
       </c>
     </row>
-    <row r="77" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N77" s="53">
         <v>53</v>
       </c>
@@ -13560,7 +13652,7 @@
         <v>25.663866445995502</v>
       </c>
     </row>
-    <row r="78" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N78" s="53">
         <v>54</v>
       </c>
@@ -13598,7 +13690,7 @@
         <v>25.489949018876814</v>
       </c>
     </row>
-    <row r="79" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N79" s="53">
         <v>55</v>
       </c>
@@ -13636,7 +13728,7 @@
         <v>25.319004685283812</v>
       </c>
     </row>
-    <row r="80" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="6:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N80" s="53">
         <v>56</v>
       </c>
@@ -13674,7 +13766,7 @@
         <v>25.150933502119997</v>
       </c>
     </row>
-    <row r="81" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N81" s="53">
         <v>57</v>
       </c>
@@ -13712,7 +13804,7 @@
         <v>24.985640482607891</v>
       </c>
     </row>
-    <row r="82" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N82" s="53">
         <v>58</v>
       </c>
@@ -13750,7 +13842,7 @@
         <v>24.823035273890088</v>
       </c>
     </row>
-    <row r="83" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N83" s="53">
         <v>59</v>
       </c>
@@ -13788,7 +13880,7 @@
         <v>24.663031860425679</v>
       </c>
     </row>
-    <row r="84" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N84" s="53">
         <v>60</v>
       </c>
@@ -13826,7 +13918,7 @@
         <v>24.505548290744287</v>
       </c>
     </row>
-    <row r="85" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N85" s="53">
         <v>61</v>
       </c>
@@ -13864,7 +13956,7 @@
         <v>24.350506425384634</v>
       </c>
     </row>
-    <row r="86" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N86" s="53">
         <v>62</v>
       </c>
@@ -13902,7 +13994,7 @@
         <v>24.197831704076748</v>
       </c>
     </row>
-    <row r="87" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N87" s="53">
         <v>63</v>
       </c>
@@ -13940,7 +14032,7 @@
         <v>24.047452930431344</v>
       </c>
     </row>
-    <row r="88" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N88" s="53">
         <v>64</v>
       </c>
@@ -13978,7 +14070,7 @@
         <v>23.899302072579939</v>
       </c>
     </row>
-    <row r="89" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N89" s="53">
         <v>65</v>
       </c>
@@ -14016,7 +14108,7 @@
         <v>23.753314078368412</v>
       </c>
     </row>
-    <row r="90" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N90" s="53">
         <v>66</v>
       </c>
@@ -14054,7 +14146,7 @@
         <v>23.609426703847415</v>
       </c>
     </row>
-    <row r="91" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N91" s="53">
         <v>67</v>
       </c>
@@ -14092,7 +14184,7 @@
         <v>23.46758035392785</v>
       </c>
     </row>
-    <row r="92" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N92" s="53">
         <v>68</v>
       </c>
@@ -14130,7 +14222,7 @@
         <v>23.327717934180452</v>
       </c>
     </row>
-    <row r="93" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N93" s="53">
         <v>69</v>
       </c>
@@ -14168,7 +14260,7 @@
         <v>23.18978471285709</v>
       </c>
     </row>
-    <row r="94" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N94" s="53">
         <v>70</v>
       </c>
@@ -14206,7 +14298,7 @@
         <v>23.053728192299307</v>
       </c>
     </row>
-    <row r="95" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N95" s="53">
         <v>71</v>
       </c>
@@ -14244,7 +14336,7 @@
         <v>22.919497988977898</v>
       </c>
     </row>
-    <row r="96" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N96" s="53">
         <v>72</v>
       </c>
@@ -14282,7 +14374,7 @@
         <v>22.787045721477696</v>
       </c>
     </row>
-    <row r="97" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N97" s="53">
         <v>73</v>
       </c>
@@ -14320,7 +14412,7 @@
         <v>22.656324905804169</v>
       </c>
     </row>
-    <row r="98" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N98" s="53">
         <v>74</v>
       </c>
@@ -14358,7 +14450,7 @@
         <v>22.527290857445088</v>
       </c>
     </row>
-    <row r="99" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N99" s="53">
         <v>75</v>
       </c>
@@ -14396,7 +14488,7 @@
         <v>22.39990059967079</v>
       </c>
     </row>
-    <row r="100" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N100" s="53">
         <v>76</v>
       </c>
@@ -14434,7 +14526,7 @@
         <v>22.274112777602188</v>
       </c>
     </row>
-    <row r="101" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N101" s="53">
         <v>77</v>
       </c>
@@ -14472,7 +14564,7 @@
         <v>22.149887577616617</v>
       </c>
     </row>
-    <row r="102" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N102" s="53">
         <v>78</v>
       </c>
@@ -14510,7 +14602,7 @@
         <v>22.027186651698472</v>
       </c>
     </row>
-    <row r="103" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N103" s="53">
         <v>79</v>
       </c>
@@ -14548,7 +14640,7 @@
         <v>21.905973046375024</v>
       </c>
     </row>
-    <row r="104" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N104" s="53">
         <v>80</v>
       </c>
@@ -14586,7 +14678,7 @@
         <v>21.786211135907866</v>
       </c>
     </row>
-    <row r="105" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N105" s="53">
         <v>81</v>
       </c>
@@ -14624,7 +14716,7 @@
         <v>21.66786655943784</v>
       </c>
     </row>
-    <row r="106" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N106" s="53">
         <v>82</v>
       </c>
@@ -14662,7 +14754,7 @@
         <v>21.550906161805923</v>
       </c>
     </row>
-    <row r="107" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N107" s="53">
         <v>83</v>
       </c>
@@ -14700,7 +14792,7 @@
         <v>21.435297937795163</v>
       </c>
     </row>
-    <row r="108" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N108" s="53">
         <v>84</v>
       </c>
@@ -14738,7 +14830,7 @@
         <v>21.321010979558935</v>
       </c>
     </row>
-    <row r="109" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N109" s="53">
         <v>85</v>
       </c>
@@ -14776,7 +14868,7 @@
         <v>21.208015427019603</v>
       </c>
     </row>
-    <row r="110" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N110" s="53">
         <v>86</v>
       </c>
@@ -14814,7 +14906,7 @@
         <v>21.096282421038353</v>
       </c>
     </row>
-    <row r="111" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N111" s="53">
         <v>87</v>
       </c>
@@ -14852,7 +14944,7 @@
         <v>20.985784059172502</v>
       </c>
     </row>
-    <row r="112" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N112" s="53">
         <v>88</v>
       </c>
@@ -14890,7 +14982,7 @@
         <v>20.876493353850599</v>
       </c>
     </row>
-    <row r="113" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N113" s="53">
         <v>89</v>
       </c>
@@ -14928,7 +15020,7 @@
         <v>20.768384192808441</v>
       </c>
     </row>
-    <row r="114" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N114" s="53">
         <v>90</v>
       </c>
@@ -14966,7 +15058,7 @@
         <v>20.661431301640963</v>
       </c>
     </row>
-    <row r="115" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N115" s="53">
         <v>91</v>
       </c>
@@ -15004,7 +15096,7 @@
         <v>20.555610208335597</v>
       </c>
     </row>
-    <row r="116" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N116" s="53">
         <v>92</v>
       </c>
@@ -15042,7 +15134,7 @@
         <v>20.450897209662639</v>
       </c>
     </row>
-    <row r="117" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N117" s="53">
         <v>93</v>
       </c>
@@ -15080,7 +15172,7 @@
         <v>20.347269339307175</v>
       </c>
     </row>
-    <row r="118" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N118" s="53">
         <v>94</v>
       </c>
@@ -15118,7 +15210,7 @@
         <v>20.244704337635284</v>
       </c>
     </row>
-    <row r="119" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N119" s="53">
         <v>95</v>
       </c>
@@ -15156,7 +15248,7 @@
         <v>20.143180622995107</v>
       </c>
     </row>
-    <row r="120" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N120" s="53">
         <v>96</v>
       </c>
@@ -15194,7 +15286,7 @@
         <v>20.042677264460092</v>
       </c>
     </row>
-    <row r="121" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N121" s="53">
         <v>97</v>
       </c>
@@ -15232,7 +15324,7 @@
         <v>19.943173955928412</v>
       </c>
     </row>
-    <row r="122" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N122" s="53">
         <v>98</v>
       </c>
@@ -15270,7 +15362,7 @@
         <v>19.844650991498295</v>
       </c>
     </row>
-    <row r="123" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N123" s="53">
         <v>99</v>
       </c>
@@ -15308,7 +15400,7 @@
         <v>19.747089242044652</v>
       </c>
     </row>
-    <row r="124" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N124" s="53">
         <v>100</v>
       </c>
@@ -15346,7 +15438,7 @@
         <v>19.650470132927282</v>
       </c>
     </row>
-    <row r="125" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="14:28" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N125" s="53">
         <v>101</v>
       </c>
@@ -15387,12 +15479,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="9NOS8jY5Ug7YrOY49rx7A6/cXCpIjF5Enxg4kw2PLmKKvG06duBf92zLgkT/MBeWCI1tXrFRs+R4hrI9dhXplw==" saltValue="nRjJWJch2cTa6A5Bi+wDuA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="22">
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="B2:AB2"/>
@@ -15409,6 +15495,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15418,73 +15510,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1E6C65-06A5-4DD3-B3AB-3E980D2AF55D}">
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AB125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="0.85546875" style="228" customWidth="1"/>
-    <col min="5" max="14" width="11.42578125" style="228"/>
-    <col min="15" max="15" width="0.5703125" style="228" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="228"/>
-    <col min="17" max="17" width="0.5703125" style="228" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="228"/>
-    <col min="19" max="19" width="0.5703125" style="228" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="228"/>
-    <col min="21" max="21" width="0.5703125" style="228" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="228"/>
-    <col min="23" max="23" width="0.5703125" style="228" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" style="228"/>
-    <col min="25" max="25" width="0.5703125" style="228" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="228"/>
-    <col min="27" max="27" width="0.5703125" style="228" customWidth="1"/>
-    <col min="28" max="16384" width="11.42578125" style="228"/>
+    <col min="1" max="4" width="0.81640625" style="198" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="198" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="198" bestFit="1" customWidth="1"/>
+    <col min="7" max="14" width="11.453125" style="198"/>
+    <col min="15" max="15" width="0.54296875" style="198" customWidth="1"/>
+    <col min="16" max="16" width="11.453125" style="198"/>
+    <col min="17" max="17" width="0.54296875" style="198" customWidth="1"/>
+    <col min="18" max="18" width="11.453125" style="198"/>
+    <col min="19" max="19" width="0.54296875" style="198" customWidth="1"/>
+    <col min="20" max="20" width="11.453125" style="198"/>
+    <col min="21" max="21" width="0.54296875" style="198" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" style="198"/>
+    <col min="23" max="23" width="0.54296875" style="198" customWidth="1"/>
+    <col min="24" max="24" width="11.453125" style="198"/>
+    <col min="25" max="25" width="0.54296875" style="198" customWidth="1"/>
+    <col min="26" max="26" width="11.453125" style="198"/>
+    <col min="27" max="27" width="0.54296875" style="198" customWidth="1"/>
+    <col min="28" max="16384" width="11.453125" style="198"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="232"/>
-      <c r="B2" s="229" t="s">
+    <row r="1" spans="1:28" ht="7" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="200"/>
+      <c r="B2" s="231" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="229"/>
-      <c r="D2" s="229"/>
-      <c r="E2" s="229"/>
-      <c r="F2" s="229"/>
-      <c r="G2" s="229"/>
-      <c r="H2" s="229"/>
-      <c r="I2" s="229"/>
-      <c r="J2" s="229"/>
-      <c r="K2" s="229"/>
-      <c r="L2" s="229"/>
-      <c r="M2" s="229"/>
-      <c r="N2" s="229"/>
-      <c r="O2" s="229"/>
-      <c r="P2" s="229"/>
-      <c r="Q2" s="229"/>
-      <c r="R2" s="229"/>
-      <c r="S2" s="229"/>
-      <c r="T2" s="229"/>
-      <c r="U2" s="229"/>
-      <c r="V2" s="229"/>
-      <c r="W2" s="229"/>
-      <c r="X2" s="229"/>
-      <c r="Y2" s="229"/>
-      <c r="Z2" s="229"/>
-      <c r="AA2" s="229"/>
-      <c r="AB2" s="229"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="231" t="s">
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="231"/>
+      <c r="H2" s="231"/>
+      <c r="I2" s="231"/>
+      <c r="J2" s="231"/>
+      <c r="K2" s="231"/>
+      <c r="L2" s="231"/>
+      <c r="M2" s="231"/>
+      <c r="N2" s="231"/>
+      <c r="O2" s="231"/>
+      <c r="P2" s="231"/>
+      <c r="Q2" s="231"/>
+      <c r="R2" s="231"/>
+      <c r="S2" s="231"/>
+      <c r="T2" s="231"/>
+      <c r="U2" s="231"/>
+      <c r="V2" s="231"/>
+      <c r="W2" s="231"/>
+      <c r="X2" s="231"/>
+      <c r="Y2" s="231"/>
+      <c r="Z2" s="231"/>
+      <c r="AA2" s="231"/>
+      <c r="AB2" s="231"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B4" s="229" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="231"/>
-      <c r="D4" s="231"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="231"/>
+      <c r="C4" s="229"/>
+      <c r="D4" s="229"/>
+      <c r="E4" s="229"/>
+      <c r="F4" s="229"/>
       <c r="G4" s="230" t="s">
         <v>23</v>
       </c>
@@ -15494,37 +15588,805 @@
       <c r="K4" s="230"/>
       <c r="L4" s="230"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="231"/>
-      <c r="C5" s="231"/>
-      <c r="D5" s="231"/>
-      <c r="E5" s="231"/>
-      <c r="F5" s="231"/>
-      <c r="G5" s="234" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B5" s="229"/>
+      <c r="C5" s="229"/>
+      <c r="D5" s="229"/>
+      <c r="E5" s="229"/>
+      <c r="F5" s="229"/>
+      <c r="G5" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="235" t="s">
+      <c r="H5" s="203" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="235" t="s">
+      <c r="I5" s="203" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="235" t="s">
+      <c r="J5" s="203" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="235" t="s">
+      <c r="K5" s="203" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="233" t="s">
+      <c r="L5" s="201" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="0.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:28" ht="0.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B7" s="237" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="237"/>
+      <c r="D7" s="237"/>
+      <c r="E7" s="237"/>
+      <c r="F7" s="198" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="238">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="239">
+        <v>5</v>
+      </c>
+      <c r="I7" s="238">
+        <v>-25</v>
+      </c>
+      <c r="J7" s="238">
+        <v>50</v>
+      </c>
+      <c r="K7" s="238"/>
+      <c r="L7" s="238"/>
+    </row>
+    <row r="8" spans="1:28" ht="0.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="238"/>
+      <c r="H8" s="238"/>
+      <c r="I8" s="238"/>
+      <c r="J8" s="238"/>
+      <c r="K8" s="238"/>
+      <c r="L8" s="238"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B9" s="237" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="237"/>
+      <c r="D9" s="237"/>
+      <c r="E9" s="237"/>
+      <c r="F9" s="198" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="238">
+        <v>-4</v>
+      </c>
+      <c r="H9" s="238">
+        <v>10</v>
+      </c>
+      <c r="I9" s="238"/>
+      <c r="J9" s="238"/>
+      <c r="K9" s="238"/>
+      <c r="L9" s="238"/>
+    </row>
+    <row r="10" spans="1:28" ht="0.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="238"/>
+      <c r="H10" s="238"/>
+      <c r="I10" s="238"/>
+      <c r="J10" s="238"/>
+      <c r="K10" s="238"/>
+      <c r="L10" s="238"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B11" s="237" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="237"/>
+      <c r="D11" s="237"/>
+      <c r="E11" s="237"/>
+      <c r="F11" s="198" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="238">
+        <v>0.5</v>
+      </c>
+      <c r="H11" s="238">
+        <v>3</v>
+      </c>
+      <c r="I11" s="238">
+        <v>-25</v>
+      </c>
+      <c r="J11" s="238"/>
+      <c r="K11" s="238"/>
+      <c r="L11" s="238"/>
+    </row>
+    <row r="12" spans="1:28" ht="0.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="238"/>
+      <c r="H12" s="238"/>
+      <c r="I12" s="238"/>
+      <c r="J12" s="238"/>
+      <c r="K12" s="238"/>
+      <c r="L12" s="238"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B13" s="237" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="237"/>
+      <c r="D13" s="237"/>
+      <c r="E13" s="237"/>
+      <c r="F13" s="198" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="238">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H13" s="238">
+        <v>0.25</v>
+      </c>
+      <c r="I13" s="238">
+        <v>-3</v>
+      </c>
+      <c r="J13" s="238">
+        <v>0</v>
+      </c>
+      <c r="K13" s="238"/>
+      <c r="L13" s="238"/>
+    </row>
+    <row r="14" spans="1:28" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="238"/>
+      <c r="H14" s="238"/>
+      <c r="I14" s="238"/>
+      <c r="J14" s="238"/>
+      <c r="K14" s="238"/>
+      <c r="L14" s="238"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B15" s="237" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="237"/>
+      <c r="D15" s="237"/>
+      <c r="E15" s="237"/>
+      <c r="F15" s="198" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="238">
+        <v>1</v>
+      </c>
+      <c r="H15" s="238">
+        <v>2</v>
+      </c>
+      <c r="I15" s="238">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="238">
+        <v>0</v>
+      </c>
+      <c r="K15" s="238">
+        <v>-20</v>
+      </c>
+      <c r="L15" s="238"/>
+    </row>
+    <row r="16" spans="1:28" ht="0.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="238"/>
+      <c r="H16" s="238"/>
+      <c r="I16" s="238"/>
+      <c r="J16" s="238"/>
+      <c r="K16" s="238"/>
+      <c r="L16" s="238"/>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="B17" s="237" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="237"/>
+      <c r="D17" s="237"/>
+      <c r="E17" s="237"/>
+      <c r="F17" s="198" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="238">
+        <v>-10</v>
+      </c>
+      <c r="H17" s="238">
+        <v>1</v>
+      </c>
+      <c r="I17" s="238">
+        <v>11</v>
+      </c>
+      <c r="J17" s="238">
+        <v>50</v>
+      </c>
+      <c r="K17" s="238"/>
+      <c r="L17" s="238"/>
+    </row>
+    <row r="18" spans="2:28" ht="2.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="B20" s="243" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="243"/>
+      <c r="D20" s="243"/>
+      <c r="E20" s="243"/>
+      <c r="F20" s="243"/>
+      <c r="G20" s="242" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="242"/>
+      <c r="I20" s="242" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="242"/>
+      <c r="K20" s="242" t="s">
+        <v>36</v>
+      </c>
+      <c r="L20" s="242"/>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="B21" s="243"/>
+      <c r="C21" s="243"/>
+      <c r="D21" s="243"/>
+      <c r="E21" s="243"/>
+      <c r="F21" s="243"/>
+      <c r="G21" s="241">
+        <v>-10</v>
+      </c>
+      <c r="H21" s="241"/>
+      <c r="I21" s="241">
+        <v>0.2</v>
+      </c>
+      <c r="J21" s="241"/>
+      <c r="K21" s="240">
+        <v>10</v>
+      </c>
+      <c r="L21" s="240"/>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="P24" s="199" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" s="199" t="s">
+        <v>15</v>
+      </c>
+      <c r="T24" s="199" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24" s="199" t="s">
+        <v>48</v>
+      </c>
+      <c r="X24" s="199" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z24" s="199" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB24" s="199" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N25" s="244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N26" s="244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N27" s="244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N28" s="244">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N29" s="244">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N30" s="244">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N31" s="244">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.35">
+      <c r="N32" s="244">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N33" s="244">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N34" s="244">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N35" s="244">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N36" s="244">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N37" s="244">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N38" s="244">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N39" s="244">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N40" s="244">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N41" s="244">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N42" s="244">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N43" s="244">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N44" s="244">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N45" s="244">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N46" s="244">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N47" s="244">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N48" s="244">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N49" s="244">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N50" s="244">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N51" s="244">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N52" s="244">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N53" s="244">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N54" s="244">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N55" s="244">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N56" s="244">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N57" s="244">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N58" s="244">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N59" s="244">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N60" s="244">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N61" s="244">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N62" s="244">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N63" s="244">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N64" s="244">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N65" s="244">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N66" s="244">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="67" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N67" s="244">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N68" s="244">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N69" s="244">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N70" s="244">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N71" s="244">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N72" s="244">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N73" s="244">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="74" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N74" s="244">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N75" s="244">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N76" s="244">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N77" s="244">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N78" s="244">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="79" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N79" s="244">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N80" s="244">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N81" s="244">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N82" s="244">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N83" s="244">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N84" s="244">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N85" s="244">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N86" s="244">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="87" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N87" s="244">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N88" s="244">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N89" s="244">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N90" s="244">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="91" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N91" s="244">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N92" s="244">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N93" s="244">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="94" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N94" s="244">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N95" s="244">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="96" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N96" s="244">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="97" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N97" s="244">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N98" s="244">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="99" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N99" s="244">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="100" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N100" s="244">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="101" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N101" s="244">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="102" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N102" s="244">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="103" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N103" s="244">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="104" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N104" s="244">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="105" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N105" s="244">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="106" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N106" s="244">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="107" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N107" s="244">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="108" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N108" s="244">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="109" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N109" s="244">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="110" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N110" s="244">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="111" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N111" s="244">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="112" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N112" s="244">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="113" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N113" s="244">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="114" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N114" s="244">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="115" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N115" s="244">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="116" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N116" s="244">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="117" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N117" s="244">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="118" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N118" s="244">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="119" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N119" s="244">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="120" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N120" s="244">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N121" s="244">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="122" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N122" s="244">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="123" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N123" s="244">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="124" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N124" s="244">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="125" spans="14:14" x14ac:dyDescent="0.35">
+      <c r="N125" s="244">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="16">
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B20:F21"/>
     <mergeCell ref="B4:F5"/>
     <mergeCell ref="G4:L4"/>
     <mergeCell ref="B2:AB2"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15539,41 +16401,41 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="0.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="1.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="0.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" style="4" customWidth="1"/>
-    <col min="7" max="10" width="11.140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0.5703125" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="0.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="0.5703125" style="33" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="0.5703125" style="33" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="1.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="0.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="1.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="0.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.26953125" style="4" customWidth="1"/>
+    <col min="7" max="10" width="11.1796875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="2.7265625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3.26953125" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0.54296875" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="0.7265625" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="0.54296875" style="33" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="0.54296875" style="33" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="11.1796875" style="2" hidden="1" customWidth="1"/>
+    <col min="21" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="201" t="s">
+    <row r="1" spans="2:21" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="213" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="201"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="201"/>
-      <c r="I2" s="201"/>
-      <c r="J2" s="201"/>
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
+      <c r="G2" s="213"/>
+      <c r="H2" s="213"/>
+      <c r="I2" s="213"/>
+      <c r="J2" s="213"/>
       <c r="K2" s="70"/>
       <c r="L2" s="70"/>
       <c r="M2" s="70"/>
@@ -15585,20 +16447,20 @@
       <c r="S2" s="70"/>
       <c r="T2" s="70"/>
     </row>
-    <row r="3" spans="2:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:21" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:21" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="29"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="202" t="s">
+      <c r="E4" s="214" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="202"/>
-      <c r="G4" s="204" t="s">
+      <c r="F4" s="214"/>
+      <c r="G4" s="216" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="205"/>
-      <c r="I4" s="205"/>
-      <c r="J4" s="205"/>
+      <c r="H4" s="217"/>
+      <c r="I4" s="217"/>
+      <c r="J4" s="217"/>
       <c r="K4" s="56"/>
       <c r="L4" s="54"/>
       <c r="M4" s="54"/>
@@ -15610,11 +16472,11 @@
       <c r="S4" s="54"/>
       <c r="T4" s="54"/>
     </row>
-    <row r="5" spans="2:21" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="30"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="203"/>
-      <c r="F5" s="203"/>
+      <c r="E5" s="215"/>
+      <c r="F5" s="215"/>
       <c r="G5" s="17" t="s">
         <v>16</v>
       </c>
@@ -15638,7 +16500,7 @@
       <c r="S5" s="54"/>
       <c r="T5" s="54"/>
     </row>
-    <row r="6" spans="2:21" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
@@ -15656,12 +16518,12 @@
       <c r="S6" s="54"/>
       <c r="T6" s="54"/>
     </row>
-    <row r="7" spans="2:21" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:21" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C7" s="24"/>
-      <c r="D7" s="223" t="s">
+      <c r="D7" s="232" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="223"/>
+      <c r="E7" s="232"/>
       <c r="F7" s="193" t="s">
         <v>52</v>
       </c>
@@ -15688,7 +16550,7 @@
       <c r="S7" s="62"/>
       <c r="T7" s="62"/>
     </row>
-    <row r="8" spans="2:21" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C8" s="22"/>
       <c r="D8" s="197"/>
       <c r="E8" s="109"/>
@@ -15708,12 +16570,12 @@
       <c r="S8" s="62"/>
       <c r="T8" s="62"/>
     </row>
-    <row r="9" spans="2:21" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="25"/>
-      <c r="D9" s="224" t="s">
+      <c r="D9" s="233" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="224"/>
+      <c r="E9" s="233"/>
       <c r="F9" s="195" t="s">
         <v>52</v>
       </c>
@@ -15741,7 +16603,7 @@
       <c r="T9" s="63"/>
       <c r="U9" s="22"/>
     </row>
-    <row r="10" spans="2:21" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" s="11" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="22"/>
       <c r="D10" s="197"/>
       <c r="E10" s="109"/>
@@ -15762,12 +16624,12 @@
       <c r="T10" s="63"/>
       <c r="U10" s="22"/>
     </row>
-    <row r="11" spans="2:21" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:21" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="26"/>
-      <c r="D11" s="225" t="s">
+      <c r="D11" s="234" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="225"/>
+      <c r="E11" s="234"/>
       <c r="F11" s="196" t="s">
         <v>53</v>
       </c>
@@ -15795,7 +16657,7 @@
       <c r="T11" s="64"/>
       <c r="U11" s="22"/>
     </row>
-    <row r="12" spans="2:21" s="11" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" s="11" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C12" s="22"/>
       <c r="D12" s="12"/>
       <c r="E12" s="22"/>
@@ -15816,7 +16678,7 @@
       <c r="T12" s="64"/>
       <c r="U12" s="22"/>
     </row>
-    <row r="13" spans="2:21" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K13" s="54"/>
       <c r="L13" s="54"/>
       <c r="M13" s="54"/>
@@ -15828,14 +16690,14 @@
       <c r="S13" s="54"/>
       <c r="T13" s="54"/>
     </row>
-    <row r="14" spans="2:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
-      <c r="E14" s="202" t="s">
+      <c r="E14" s="214" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="206"/>
+      <c r="F14" s="218"/>
       <c r="G14" s="71" t="s">
         <v>24</v>
       </c>
@@ -15857,12 +16719,12 @@
       <c r="S14" s="54"/>
       <c r="T14" s="54"/>
     </row>
-    <row r="15" spans="2:21" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="207"/>
-      <c r="F15" s="208"/>
+      <c r="E15" s="219"/>
+      <c r="F15" s="220"/>
       <c r="G15" s="191">
         <f>-2*PI()</f>
         <v>-6.2831853071795862</v>
@@ -15887,7 +16749,7 @@
       <c r="S15" s="54"/>
       <c r="T15" s="54"/>
     </row>
-    <row r="16" spans="2:21" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:21" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K16" s="54"/>
       <c r="L16" s="54"/>
       <c r="M16" s="54"/>
@@ -15899,7 +16761,7 @@
       <c r="S16" s="54"/>
       <c r="T16" s="54"/>
     </row>
-    <row r="17" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K17" s="54"/>
       <c r="L17" s="54"/>
       <c r="M17" s="54"/>
@@ -15911,7 +16773,7 @@
       <c r="S17" s="54"/>
       <c r="T17" s="54"/>
     </row>
-    <row r="18" spans="6:20" s="7" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:20" s="7" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -15935,7 +16797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F19" s="1"/>
       <c r="K19" s="54"/>
       <c r="L19" s="59">
@@ -15962,7 +16824,7 @@
         <v>2.45029690981724E-16</v>
       </c>
     </row>
-    <row r="20" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K20" s="54"/>
       <c r="L20" s="59">
         <v>2</v>
@@ -15988,7 +16850,7 @@
         <v>0.12632937844610859</v>
       </c>
     </row>
-    <row r="21" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K21" s="54"/>
       <c r="L21" s="59">
         <v>3</v>
@@ -16014,7 +16876,7 @@
         <v>0.25675636036772742</v>
       </c>
     </row>
-    <row r="22" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -16045,7 +16907,7 @@
         <v>0.39592800879772216</v>
       </c>
     </row>
-    <row r="23" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -16076,7 +16938,7 @@
         <v>0.54975465219277131</v>
       </c>
     </row>
-    <row r="24" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -16107,7 +16969,7 @@
         <v>0.72654252800536256</v>
       </c>
     </row>
-    <row r="25" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -16138,7 +17000,7 @@
         <v>0.93906250581749473</v>
       </c>
     </row>
-    <row r="26" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -16169,7 +17031,7 @@
         <v>1.2087923504096127</v>
       </c>
     </row>
-    <row r="27" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -16200,7 +17062,7 @@
         <v>1.5757478599686567</v>
       </c>
     </row>
-    <row r="28" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -16231,7 +17093,7 @@
         <v>2.1251081731572126</v>
       </c>
     </row>
-    <row r="29" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -16262,7 +17124,7 @@
         <v>3.077683537175274</v>
       </c>
     </row>
-    <row r="30" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -16293,7 +17155,7 @@
         <v>5.2421835811132382</v>
       </c>
     </row>
-    <row r="31" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -16324,7 +17186,7 @@
         <v>15.894544843865891</v>
       </c>
     </row>
-    <row r="32" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -16355,7 +17217,7 @@
         <v>-15.894544843864672</v>
       </c>
     </row>
-    <row r="33" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -16386,7 +17248,7 @@
         <v>-5.2421835811131006</v>
       </c>
     </row>
-    <row r="34" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -16417,7 +17279,7 @@
         <v>-3.0776835371752238</v>
       </c>
     </row>
-    <row r="35" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -16448,7 +17310,7 @@
         <v>-2.1251081731571864</v>
       </c>
     </row>
-    <row r="36" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -16479,7 +17341,7 @@
         <v>-1.5757478599686401</v>
       </c>
     </row>
-    <row r="37" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -16510,7 +17372,7 @@
         <v>-1.208792350409601</v>
       </c>
     </row>
-    <row r="38" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -16541,7 +17403,7 @@
         <v>-0.93906250581748574</v>
       </c>
     </row>
-    <row r="39" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -16572,7 +17434,7 @@
         <v>-0.72654252800535524</v>
       </c>
     </row>
-    <row r="40" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -16603,7 +17465,7 @@
         <v>-0.54975465219276498</v>
       </c>
     </row>
-    <row r="41" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -16634,7 +17496,7 @@
         <v>-0.39592800879771656</v>
       </c>
     </row>
-    <row r="42" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -16665,7 +17527,7 @@
         <v>-0.25675636036772231</v>
       </c>
     </row>
-    <row r="43" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -16696,7 +17558,7 @@
         <v>-0.1263293784461037</v>
       </c>
     </row>
-    <row r="44" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -16727,7 +17589,7 @@
         <v>4.5634069439914882E-15</v>
       </c>
     </row>
-    <row r="45" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -16758,7 +17620,7 @@
         <v>0.126329378446113</v>
       </c>
     </row>
-    <row r="46" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -16789,7 +17651,7 @@
         <v>0.25675636036773203</v>
       </c>
     </row>
-    <row r="47" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -16820,7 +17682,7 @@
         <v>0.39592800879772716</v>
       </c>
     </row>
-    <row r="48" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -16851,7 +17713,7 @@
         <v>0.54975465219277697</v>
       </c>
     </row>
-    <row r="49" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -16882,7 +17744,7 @@
         <v>0.72654252800536923</v>
       </c>
     </row>
-    <row r="50" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -16913,7 +17775,7 @@
         <v>0.93906250581750284</v>
       </c>
     </row>
-    <row r="51" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -16944,7 +17806,7 @@
         <v>1.2087923504096234</v>
       </c>
     </row>
-    <row r="52" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -16975,7 +17837,7 @@
         <v>1.5757478599686718</v>
       </c>
     </row>
-    <row r="53" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -17006,7 +17868,7 @@
         <v>2.1251081731572365</v>
       </c>
     </row>
-    <row r="54" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -17037,7 +17899,7 @@
         <v>3.0776835371753171</v>
       </c>
     </row>
-    <row r="55" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -17068,7 +17930,7 @@
         <v>5.2421835811133484</v>
       </c>
     </row>
-    <row r="56" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -17099,7 +17961,7 @@
         <v>15.894544843866818</v>
       </c>
     </row>
-    <row r="57" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -17130,7 +17992,7 @@
         <v>-15.894544843863802</v>
       </c>
     </row>
-    <row r="58" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -17161,7 +18023,7 @@
         <v>-5.2421835811130091</v>
       </c>
     </row>
-    <row r="59" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -17192,7 +18054,7 @@
         <v>-3.0776835371751923</v>
       </c>
     </row>
-    <row r="60" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -17223,7 +18085,7 @@
         <v>-2.1251081731571708</v>
       </c>
     </row>
-    <row r="61" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -17254,7 +18116,7 @@
         <v>-1.5757478599686312</v>
       </c>
     </row>
-    <row r="62" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -17285,7 +18147,7 @@
         <v>-1.2087923504095952</v>
       </c>
     </row>
-    <row r="63" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -17316,7 +18178,7 @@
         <v>-0.93906250581748174</v>
       </c>
     </row>
-    <row r="64" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -17347,7 +18209,7 @@
         <v>-0.72654252800535235</v>
       </c>
     </row>
-    <row r="65" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -17378,7 +18240,7 @@
         <v>-0.54975465219276287</v>
       </c>
     </row>
-    <row r="66" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -17409,7 +18271,7 @@
         <v>-0.39592800879771484</v>
       </c>
     </row>
-    <row r="67" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L67" s="59">
         <v>49</v>
       </c>
@@ -17432,7 +18294,7 @@
         <v>-0.25675636036772087</v>
       </c>
     </row>
-    <row r="68" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L68" s="59">
         <v>50</v>
       </c>
@@ -17455,7 +18317,7 @@
         <v>-0.12632937844610254</v>
       </c>
     </row>
-    <row r="69" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L69" s="59">
         <v>51</v>
       </c>
@@ -17478,7 +18340,7 @@
         <v>5.5511151231257827E-15</v>
       </c>
     </row>
-    <row r="70" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L70" s="59">
         <v>52</v>
       </c>
@@ -17501,7 +18363,7 @@
         <v>0.12632937844611383</v>
       </c>
     </row>
-    <row r="71" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L71" s="59">
         <v>53</v>
       </c>
@@ -17524,7 +18386,7 @@
         <v>0.25675636036773269</v>
       </c>
     </row>
-    <row r="72" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L72" s="59">
         <v>54</v>
       </c>
@@ -17547,7 +18409,7 @@
         <v>0.39592800879772772</v>
       </c>
     </row>
-    <row r="73" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L73" s="59">
         <v>55</v>
       </c>
@@ -17570,7 +18432,7 @@
         <v>0.5497546521927773</v>
       </c>
     </row>
-    <row r="74" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L74" s="59">
         <v>56</v>
       </c>
@@ -17593,7 +18455,7 @@
         <v>0.72654252800536934</v>
       </c>
     </row>
-    <row r="75" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L75" s="59">
         <v>57</v>
       </c>
@@ -17616,7 +18478,7 @@
         <v>0.93906250581750261</v>
       </c>
     </row>
-    <row r="76" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L76" s="59">
         <v>58</v>
       </c>
@@ -17639,7 +18501,7 @@
         <v>1.2087923504096225</v>
       </c>
     </row>
-    <row r="77" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L77" s="59">
         <v>59</v>
       </c>
@@ -17662,7 +18524,7 @@
         <v>1.5757478599686698</v>
       </c>
     </row>
-    <row r="78" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L78" s="59">
         <v>60</v>
       </c>
@@ -17685,7 +18547,7 @@
         <v>2.1251081731572321</v>
       </c>
     </row>
-    <row r="79" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L79" s="59">
         <v>61</v>
       </c>
@@ -17708,7 +18570,7 @@
         <v>3.0776835371753086</v>
       </c>
     </row>
-    <row r="80" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="6:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L80" s="59">
         <v>62</v>
       </c>
@@ -17731,7 +18593,7 @@
         <v>5.2421835811133253</v>
       </c>
     </row>
-    <row r="81" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L81" s="59">
         <v>63</v>
       </c>
@@ -17754,7 +18616,7 @@
         <v>15.894544843866617</v>
       </c>
     </row>
-    <row r="82" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L82" s="59">
         <v>64</v>
       </c>
@@ -17777,7 +18639,7 @@
         <v>-15.894544843864002</v>
       </c>
     </row>
-    <row r="83" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L83" s="59">
         <v>65</v>
       </c>
@@ -17800,7 +18662,7 @@
         <v>-5.2421835811130322</v>
       </c>
     </row>
-    <row r="84" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L84" s="59">
         <v>66</v>
       </c>
@@ -17823,7 +18685,7 @@
         <v>-3.0776835371752007</v>
       </c>
     </row>
-    <row r="85" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L85" s="59">
         <v>67</v>
       </c>
@@ -17846,7 +18708,7 @@
         <v>-2.1251081731571753</v>
       </c>
     </row>
-    <row r="86" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L86" s="59">
         <v>68</v>
       </c>
@@ -17869,7 +18731,7 @@
         <v>-1.5757478599686332</v>
       </c>
     </row>
-    <row r="87" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L87" s="59">
         <v>69</v>
       </c>
@@ -17892,7 +18754,7 @@
         <v>-1.2087923504095961</v>
       </c>
     </row>
-    <row r="88" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L88" s="59">
         <v>70</v>
       </c>
@@ -17915,7 +18777,7 @@
         <v>-0.93906250581748196</v>
       </c>
     </row>
-    <row r="89" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L89" s="59">
         <v>71</v>
       </c>
@@ -17938,7 +18800,7 @@
         <v>-0.72654252800535224</v>
       </c>
     </row>
-    <row r="90" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L90" s="59">
         <v>72</v>
       </c>
@@ -17961,7 +18823,7 @@
         <v>-0.54975465219276243</v>
       </c>
     </row>
-    <row r="91" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L91" s="59">
         <v>73</v>
       </c>
@@ -17984,7 +18846,7 @@
         <v>-0.39592800879771428</v>
       </c>
     </row>
-    <row r="92" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L92" s="59">
         <v>74</v>
       </c>
@@ -18007,7 +18869,7 @@
         <v>-0.2567563603677202</v>
       </c>
     </row>
-    <row r="93" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L93" s="59">
         <v>75</v>
       </c>
@@ -18030,7 +18892,7 @@
         <v>-0.1263293784461017</v>
       </c>
     </row>
-    <row r="94" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L94" s="59">
         <v>76</v>
       </c>
@@ -18053,7 +18915,7 @@
         <v>6.5388233022600772E-15</v>
       </c>
     </row>
-    <row r="95" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L95" s="59">
         <v>77</v>
       </c>
@@ -18076,7 +18938,7 @@
         <v>0.126329378446115</v>
       </c>
     </row>
-    <row r="96" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L96" s="59">
         <v>78</v>
       </c>
@@ -18099,7 +18961,7 @@
         <v>0.25675636036773414</v>
       </c>
     </row>
-    <row r="97" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L97" s="59">
         <v>79</v>
       </c>
@@ -18122,7 +18984,7 @@
         <v>0.39592800879772944</v>
       </c>
     </row>
-    <row r="98" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L98" s="59">
         <v>80</v>
       </c>
@@ -18145,7 +19007,7 @@
         <v>0.54975465219277952</v>
       </c>
     </row>
-    <row r="99" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L99" s="59">
         <v>81</v>
       </c>
@@ -18168,7 +19030,7 @@
         <v>0.72654252800537222</v>
       </c>
     </row>
-    <row r="100" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L100" s="59">
         <v>82</v>
       </c>
@@ -18191,7 +19053,7 @@
         <v>0.93906250581750661</v>
       </c>
     </row>
-    <row r="101" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L101" s="59">
         <v>83</v>
       </c>
@@ -18214,7 +19076,7 @@
         <v>1.2087923504096272</v>
       </c>
     </row>
-    <row r="102" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L102" s="59">
         <v>84</v>
       </c>
@@ -18237,7 +19099,7 @@
         <v>1.5757478599686772</v>
       </c>
     </row>
-    <row r="103" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L103" s="59">
         <v>85</v>
       </c>
@@ -18260,7 +19122,7 @@
         <v>2.125108173157245</v>
       </c>
     </row>
-    <row r="104" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L104" s="59">
         <v>86</v>
       </c>
@@ -18283,7 +19145,7 @@
         <v>3.0776835371753353</v>
       </c>
     </row>
-    <row r="105" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L105" s="59">
         <v>87</v>
       </c>
@@ -18306,7 +19168,7 @@
         <v>5.2421835811134043</v>
       </c>
     </row>
-    <row r="106" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L106" s="59">
         <v>88</v>
       </c>
@@ -18329,7 +19191,7 @@
         <v>15.894544843867376</v>
       </c>
     </row>
-    <row r="107" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L107" s="59">
         <v>89</v>
       </c>
@@ -18352,7 +19214,7 @@
         <v>-15.894544843863189</v>
       </c>
     </row>
-    <row r="108" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L108" s="59">
         <v>90</v>
       </c>
@@ -18375,7 +19237,7 @@
         <v>-5.2421835811129345</v>
       </c>
     </row>
-    <row r="109" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L109" s="59">
         <v>91</v>
       </c>
@@ -18398,7 +19260,7 @@
         <v>-3.0776835371751625</v>
       </c>
     </row>
-    <row r="110" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L110" s="59">
         <v>92</v>
       </c>
@@ -18421,7 +19283,7 @@
         <v>-2.1251081731571539</v>
       </c>
     </row>
-    <row r="111" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L111" s="59">
         <v>93</v>
       </c>
@@ -18444,7 +19306,7 @@
         <v>-1.5757478599686197</v>
       </c>
     </row>
-    <row r="112" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L112" s="59">
         <v>94</v>
       </c>
@@ -18467,7 +19329,7 @@
         <v>-1.2087923504095865</v>
       </c>
     </row>
-    <row r="113" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L113" s="59">
         <v>95</v>
       </c>
@@ -18490,7 +19352,7 @@
         <v>-0.93906250581747475</v>
       </c>
     </row>
-    <row r="114" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L114" s="59">
         <v>96</v>
       </c>
@@ -18513,7 +19375,7 @@
         <v>-0.72654252800534624</v>
       </c>
     </row>
-    <row r="115" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L115" s="59">
         <v>97</v>
       </c>
@@ -18536,7 +19398,7 @@
         <v>-0.54975465219275743</v>
       </c>
     </row>
-    <row r="116" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L116" s="59">
         <v>98</v>
       </c>
@@ -18559,7 +19421,7 @@
         <v>-0.39592800879770984</v>
       </c>
     </row>
-    <row r="117" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L117" s="59">
         <v>99</v>
       </c>
@@ -18582,7 +19444,7 @@
         <v>-0.25675636036771604</v>
       </c>
     </row>
-    <row r="118" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L118" s="59">
         <v>100</v>
       </c>
@@ -18605,7 +19467,7 @@
         <v>-0.12632937844609776</v>
       </c>
     </row>
-    <row r="119" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="12:20" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L119" s="59">
         <v>101</v>
       </c>
@@ -18656,109 +19518,109 @@
       <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="11" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="1.7265625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="2.7265625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="33.26953125" style="11" customWidth="1"/>
     <col min="4" max="4" width="100" style="11" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="11"/>
+    <col min="5" max="5" width="1.7265625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:4" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="226" t="s">
+    <row r="1" spans="2:4" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:4" ht="13" x14ac:dyDescent="0.35">
+      <c r="B2" s="235" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-    </row>
-    <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="227" t="s">
+      <c r="C2" s="235"/>
+      <c r="D2" s="235"/>
+    </row>
+    <row r="3" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="236" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="75" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="227"/>
+    <row r="5" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="236"/>
       <c r="D5" s="76" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="227"/>
+    <row r="6" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="236"/>
       <c r="D6" s="77" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="227"/>
+    <row r="7" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="236"/>
       <c r="D7" s="76" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="227"/>
+    <row r="8" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="236"/>
       <c r="D8" s="77" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="227"/>
+    <row r="9" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="236"/>
       <c r="D9" s="78" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="227" t="s">
+    <row r="11" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="236" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="79" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="227"/>
+    <row r="12" spans="2:4" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="236"/>
       <c r="D12" s="76" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="227"/>
+    <row r="13" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="236"/>
       <c r="D13" s="82" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="227" t="s">
+    <row r="14" spans="2:4" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C15" s="236" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="75" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="227"/>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C16" s="236"/>
       <c r="D16" s="76" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="227"/>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="236"/>
       <c r="D17" s="81" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="227"/>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C18" s="236"/>
       <c r="D18" s="80" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Ajout du graphique trig et masquage
</commit_message>
<xml_diff>
--- a/ExerciceExcel3/Islam_Shafaatul_Excel_Exercice03_FonctionsMathematiques.xlsx
+++ b/ExerciceExcel3/Islam_Shafaatul_Excel_Exercice03_FonctionsMathematiques.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4fc197a25ccdc5fa/Desktop/GitHub2022/ExerciceExcel3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{EF801937-CD40-463B-A4F4-654C67F91411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACA22660-80A7-4C40-BFE3-897613F5D141}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="13_ncr:1_{EF801937-CD40-463B-A4F4-654C67F91411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B734D00F-E451-4FE3-9C11-3A14D76C94F8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{1DA72D1B-FF99-485E-854D-77014E075997}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{1DA72D1B-FF99-485E-854D-77014E075997}"/>
   </bookViews>
   <sheets>
     <sheet name="Fonctions mathématiques" sheetId="1" r:id="rId1"/>
@@ -1847,7 +1847,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="58">
+  <fills count="61">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2250,8 +2250,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="81">
+  <borders count="82">
     <border>
       <left/>
       <right/>
@@ -3187,11 +3205,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="260">
+  <cellXfs count="272">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
@@ -3995,6 +4024,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="37" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="38" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="45" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="46" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="49" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="50" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -4071,37 +4124,13 @@
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="37" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="38" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="45" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="46" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="49" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="50" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="45" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="56" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4111,12 +4140,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="45" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="56" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="53" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4144,6 +4173,30 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="81" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="81" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="45" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="58" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="59" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="60" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14534,7 +14587,2283 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Fonctions</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> trigonométriques</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cosinus</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fonctions trigonométrique(Ex)'!$N$6:$N$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6.2830000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.0309999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.9049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.778999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.6529999999999987</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.5269999999999984</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.400999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.2749999999999977</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.1489999999999974</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.022999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.8969999999999967</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.7709999999999964</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.644999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.5189999999999957</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.3929999999999954</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.266999999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-4.1409999999999947</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4.0149999999999944</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.8889999999999945</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.7629999999999946</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.6369999999999947</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.5109999999999948</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.3849999999999949</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.258999999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.1329999999999951</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.0069999999999952</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-2.8809999999999953</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.7549999999999955</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-2.6289999999999956</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-2.5029999999999957</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-2.3769999999999958</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-2.2509999999999959</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-2.124999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.9989999999999961</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.8729999999999962</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.7469999999999963</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.6209999999999964</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.4949999999999966</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.3689999999999967</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.2429999999999968</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.1169999999999969</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.99099999999999688</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.86499999999999688</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.73899999999999688</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.61299999999999688</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.48699999999999688</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.36099999999999688</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.23499999999999688</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.10899999999999688</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.7000000000003124E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14300000000000312</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.26900000000000313</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.39500000000000313</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.52100000000000313</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.64700000000000313</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.77300000000000313</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.89900000000000313</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.025000000000003</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.1510000000000029</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.2770000000000028</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.4030000000000027</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.5290000000000026</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.6550000000000025</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.7810000000000024</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.9070000000000022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.0330000000000021</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.159000000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.2850000000000019</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.4110000000000018</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.5370000000000017</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.6630000000000016</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.7890000000000015</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.9150000000000014</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.0410000000000013</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.1670000000000011</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.293000000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.4190000000000009</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.5450000000000008</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.6710000000000007</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.7970000000000006</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.9230000000000005</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.0490000000000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.1750000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.301000000000001</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.4270000000000014</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.5530000000000017</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.679000000000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.8050000000000024</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.9310000000000027</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.057000000000003</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.1830000000000034</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.3090000000000037</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.4350000000000041</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.5610000000000044</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.6870000000000047</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.8130000000000051</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.9390000000000054</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.0650000000000057</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.1910000000000061</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.3170000000000064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fonctions trigonométrique(Ex)'!$O$6:$O$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>1.9999998626449984</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9366464006597808</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7509576050443236</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4546631858558041</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0664796607878269</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61092805806360073</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11678495625011225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3847352932868755</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.86195233473820387</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.2847210130770723</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-1.6263356027278775</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.8652167721287753</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.9862747209183347</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.9818623822139703</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.8522584774835269</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.6056499100871529</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.2576146096656089</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.83013749539550097</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.35022171838159949</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.15181709087410353</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.64426581984642162</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0960171484101677</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.4785345561768382</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.7676549358891831</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9451149442237328</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.9997046724856242</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.9279757613783808</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.734459229196436</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.4313792535281096</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0378809864917218</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.57882118137192895</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8.3198025135866147E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.4176806378147449</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.89217497982759986</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.3103118351167158</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.6456780641035582</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.8770890357179211</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.9899268318883914</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.97706364165479</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.8393120153454783</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.5853735368721693</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.2312891564439479</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.79942590543948244</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.31706400128838325</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.18532640696472361</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.67600999676155527</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.1239909494311202</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.5009709141303569</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.7831365763906635</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.9526639129830954</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.9988441113570419</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.9187600308443546</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.7174704744896434</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.4076906313044633</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.0089888749759628</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.54655065616916398</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.9587571674182825E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-0.45050789265152419</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-0.92214538275343649</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-1.3355321963166202</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-1.6645552474734828</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-1.888430595117583</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-1.993016336351058</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-1.9717059313624044</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-1.8258455296103953</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-1.5646489353835642</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-1.204615584245851</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-0.76848829600909074</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-0.28381664156733977</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.2187833262330737</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.70756304724071273</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.151646967600835</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.5229829067302567</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.7981140756215379</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.9596608104770303</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.9974184225633183</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.909001814595692</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.6999961441075493</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.3836040166034722</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.9798114948272868</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.51412560621159842</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.5963098455566684E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-0.48320777663828612</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-0.9518550700666224</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-1.3603749661938487</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-1.6829618157438304</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-1.8992382437600548</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-1.9955423608192862</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-1.9657907661074201</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-1.8118628276205282</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-1.543481965030572</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-1.1776014344165799</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-0.73733341400903485</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-0.25048903915248522</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.25217838949694971</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.73891605037724739</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.1789773838098276</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.5445643105867863</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.8125831990348991</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.966103658492073</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.9954280091854995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-97DA-4E19-A351-0BAE812BC343}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Sinus</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fonctions trigonométrique(Ex)'!$N$6:$N$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6.2830000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.0309999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.9049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.778999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.6529999999999987</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.5269999999999984</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.400999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.2749999999999977</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.1489999999999974</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.022999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.8969999999999967</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.7709999999999964</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.644999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.5189999999999957</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.3929999999999954</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.266999999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-4.1409999999999947</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4.0149999999999944</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.8889999999999945</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.7629999999999946</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.6369999999999947</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.5109999999999948</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.3849999999999949</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.258999999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.1329999999999951</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.0069999999999952</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-2.8809999999999953</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.7549999999999955</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-2.6289999999999956</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-2.5029999999999957</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-2.3769999999999958</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-2.2509999999999959</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-2.124999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.9989999999999961</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.8729999999999962</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.7469999999999963</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.6209999999999964</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.4949999999999966</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.3689999999999967</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.2429999999999968</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.1169999999999969</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.99099999999999688</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.86499999999999688</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.73899999999999688</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.61299999999999688</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.48699999999999688</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.36099999999999688</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.23499999999999688</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.10899999999999688</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.7000000000003124E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14300000000000312</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.26900000000000313</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.39500000000000313</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.52100000000000313</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.64700000000000313</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.77300000000000313</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.89900000000000313</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.025000000000003</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.1510000000000029</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.2770000000000028</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.4030000000000027</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.5290000000000026</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.6550000000000025</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.7810000000000024</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.9070000000000022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.0330000000000021</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.159000000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.2850000000000019</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.4110000000000018</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.5370000000000017</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.6630000000000016</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.7890000000000015</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.9150000000000014</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.0410000000000013</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.1670000000000011</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.293000000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.4190000000000009</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.5450000000000008</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.6710000000000007</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.7970000000000006</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.9230000000000005</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.0490000000000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.1750000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.301000000000001</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.4270000000000014</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.5530000000000017</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.679000000000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.8050000000000024</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.9310000000000027</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.057000000000003</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.1830000000000034</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.3090000000000037</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.4350000000000041</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.5610000000000044</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.6870000000000047</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.8130000000000051</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.9390000000000054</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.0650000000000057</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.1910000000000061</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.3170000000000064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fonctions trigonométrique(Ex)'!$P$6:$P$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>3.7061435705115694E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25170140909462396</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.49904147618777767</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.73846923710077184</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.96618856296903721</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1785889622495196</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3723028250899609</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5442588168072331</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6917305739207422</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8123799306649455</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9042939906243146</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9660154557197091</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.99656573167986</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9954604436605528</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9627171160112522</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8988548944264154</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8048863148867877</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.6823012498941743</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.533043286532249</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.359478910879421</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1643599873551043</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.95078012788963584</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.72212564268495683</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.48202185024209948</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.23427559791038235</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-1.7185095704586758E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.26837331950404325</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.51530648240009946</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.75406945732597497</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.98087665560368908</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-1.1921320474796704</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-1.3844861772022623</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.5548892686666613</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.7006395796369083</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.8194262378883943</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.909365880103538</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.9690325126106782</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.9974801205239545</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.9942576668160987</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.9594162435137354</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.8935082616329324</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.7975786926985833</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.6731485007133953</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.5221905272627285</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1.3470982120971271</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1.1506476451279275</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.93595355150182513</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.70641990761136042</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.46568597102482751</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.21756858003145702</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.3998362357003702E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.28502626046672513</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.531535065174779</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.76961637761649582</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.99549541687746468</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.2055908691719741</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.3965716695987418</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.5654098161987884</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.7094283789481899</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.8263439425027861</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.9143028097648196</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.9719103922637009</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.9982533213662022</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.9929139297426781</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9559768734855725</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.8880277898864637</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.790144012152612</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.6638774882812408</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.5112301749129216</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.3346222962946956</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.1368539716072981</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.92106081905548731</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.69066424061894449</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.44931717569937385</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.20084618374011914</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-5.0809225901225066E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-0.30165905490190098</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-0.54772607742598001</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-0.78510889906848458</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-1.0100438134916292</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-1.2189644760157703</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-1.408558448039851</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-1.5758197157791516</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-1.7180963506353835</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-1.8331325555436107</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-1.919104430650878</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-1.9746488912614453</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-1.9988852795544036</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-1.9914293274197354</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-1.9523992490319515</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-1.8824138665635068</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-1.7825827987548235</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-1.6544888679012122</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-1.5001630041940393</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-1.322052045307994</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-1.1229799417722262</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-0.90610298321447569</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-0.67485975536641218</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.43291662126222519</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-0.18410959102645097</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.7616498094034305E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-97DA-4E19-A351-0BAE812BC343}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Tangente</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Fonctions trigonométrique(Ex)'!$N$6:$N$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6.2830000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.0309999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.9049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.778999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.6529999999999987</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.5269999999999984</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.400999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.2749999999999977</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.1489999999999974</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.022999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.8969999999999967</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.7709999999999964</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.644999999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.5189999999999957</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.3929999999999954</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.266999999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-4.1409999999999947</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-4.0149999999999944</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.8889999999999945</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.7629999999999946</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.6369999999999947</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.5109999999999948</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.3849999999999949</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.258999999999995</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-3.1329999999999951</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.0069999999999952</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-2.8809999999999953</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.7549999999999955</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-2.6289999999999956</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-2.5029999999999957</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-2.3769999999999958</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-2.2509999999999959</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-2.124999999999996</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.9989999999999961</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.8729999999999962</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.7469999999999963</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.6209999999999964</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.4949999999999966</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.3689999999999967</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.2429999999999968</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.1169999999999969</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.99099999999999688</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.86499999999999688</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.73899999999999688</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.61299999999999688</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.48699999999999688</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.36099999999999688</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.23499999999999688</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.10899999999999688</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.7000000000003124E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14300000000000312</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.26900000000000313</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.39500000000000313</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.52100000000000313</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.64700000000000313</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.77300000000000313</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.89900000000000313</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.025000000000003</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.1510000000000029</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.2770000000000028</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.4030000000000027</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.5290000000000026</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.6550000000000025</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.7810000000000024</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.9070000000000022</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.0330000000000021</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.159000000000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.2850000000000019</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.4110000000000018</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.5370000000000017</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.6630000000000016</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.7890000000000015</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.9150000000000014</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.0410000000000013</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.1670000000000011</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.293000000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.4190000000000009</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.5450000000000008</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.6710000000000007</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.7970000000000006</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.9230000000000005</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>4.0490000000000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.1750000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.301000000000001</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.4270000000000014</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.5530000000000017</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.679000000000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.8050000000000024</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.9310000000000027</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5.057000000000003</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>5.1830000000000034</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.3090000000000037</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.4350000000000041</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.5610000000000044</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.6870000000000047</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.8130000000000051</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.9390000000000054</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.0650000000000057</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.1910000000000061</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.3170000000000064</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Fonctions trigonométrique(Ex)'!$Q$6:$Q$106</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>1.8530718170718704E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12685933874040059</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25767101267078973</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39731005147085796</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.55174937272282631</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72939858560826298</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94321692959671877</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2150614368902624</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5858093426187767</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.1429473993321628</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1152516648024537</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3551174609773442</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.042096526443199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-14.816751605132295</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-5.106301155025827</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-3.0237842894140581</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.0947642028376494</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.5553794504950544</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.193552774307163</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.9267653727245575</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.71603576798111146</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.54035405793876157</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.38718150715586014</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.24833113019580119</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.1179498042086834</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.5928650718340941E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.13541130963318615</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.26665623604500688</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.40707739810346705</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.5627675154822025</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.74235860794953468</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.95923131106856674</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.2360965520547245</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.6157594239734745</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.1908269093209292</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.2076733614779225</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.6163940982019902</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>19.902123863539483</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-13.167976346854354</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-4.8880428238793456</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.9406185723143499</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-2.0502480520082926</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1.5270034016933942</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1.1733706337693091</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.91125747300289139</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.70339372111986542</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.52954078276503691</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.37754496102267854</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.23942370370944582</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.10943373774527267</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.7001637856006207E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.14398277515784177</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.27568183832459875</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.41691183224909656</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.57389041844288291</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.75548142405864793</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.97550609757446871</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.2575734751398955</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.6465344294765589</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.2405033486537196</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.3052182004054793</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.903568646087118</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>23.911613719025262</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-11.847885307064628</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-4.6870156339738278</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-2.8614659143282859</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-2.0072405939160722</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-1.499346720636185</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-1.1535828036201592</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-0.89598539218629791</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-0.69090032061945306</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-0.51882336520009686</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-0.36796939846559823</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-0.2305520658652129</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-0.10093332761480862</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.5412814917901309E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.15257501806538845</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.28474937701885827</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.4268154523167666</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.58512117803174768</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.7687720113361487</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.99205005061325846</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.2795094068958039</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.6781734518083602</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.2920872422041083</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.4083392987317778</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.2207395900259765</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>29.938870635093895</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-10.766963094173494</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-4.5012312539459511</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-2.7860322782578582</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-1.9656606301622808</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-1.4723786298540331</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-1.1341751228437211</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-0.88094168135166395</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-0.67855122459655814</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-0.50819904096448887</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-0.35845290137796304</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-0.22171475463619375</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-9.2447332172630389E-2</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3.3827587001537422E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-97DA-4E19-A351-0BAE812BC343}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1363448847"/>
+        <c:axId val="1363448431"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1363448847"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1363448431"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1363448431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="-5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1363448847"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -15090,6 +17419,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15213,6 +18058,51 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>774699</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5236FB83-A83F-F5B8-7793-90577D99B70C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15571,52 +18461,52 @@
   <sheetData>
     <row r="1" spans="2:29" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="229" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
-      <c r="J2" s="223"/>
-      <c r="K2" s="223"/>
-      <c r="L2" s="223"/>
-      <c r="M2" s="223"/>
-      <c r="N2" s="223"/>
-      <c r="O2" s="223"/>
-      <c r="P2" s="223"/>
-      <c r="Q2" s="223"/>
-      <c r="R2" s="223"/>
-      <c r="S2" s="223"/>
-      <c r="T2" s="223"/>
-      <c r="U2" s="223"/>
-      <c r="V2" s="223"/>
-      <c r="W2" s="223"/>
-      <c r="X2" s="223"/>
-      <c r="Y2" s="223"/>
-      <c r="Z2" s="223"/>
-      <c r="AA2" s="223"/>
-      <c r="AB2" s="223"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="229"/>
+      <c r="I2" s="229"/>
+      <c r="J2" s="229"/>
+      <c r="K2" s="229"/>
+      <c r="L2" s="229"/>
+      <c r="M2" s="229"/>
+      <c r="N2" s="229"/>
+      <c r="O2" s="229"/>
+      <c r="P2" s="229"/>
+      <c r="Q2" s="229"/>
+      <c r="R2" s="229"/>
+      <c r="S2" s="229"/>
+      <c r="T2" s="229"/>
+      <c r="U2" s="229"/>
+      <c r="V2" s="229"/>
+      <c r="W2" s="229"/>
+      <c r="X2" s="229"/>
+      <c r="Y2" s="229"/>
+      <c r="Z2" s="229"/>
+      <c r="AA2" s="229"/>
+      <c r="AB2" s="229"/>
     </row>
     <row r="3" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:29" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="29"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="224" t="s">
+      <c r="E4" s="230" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="224"/>
-      <c r="G4" s="226" t="s">
+      <c r="F4" s="230"/>
+      <c r="G4" s="232" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="227"/>
-      <c r="I4" s="227"/>
-      <c r="J4" s="227"/>
-      <c r="K4" s="227"/>
-      <c r="L4" s="227"/>
+      <c r="H4" s="233"/>
+      <c r="I4" s="233"/>
+      <c r="J4" s="233"/>
+      <c r="K4" s="233"/>
+      <c r="L4" s="233"/>
       <c r="M4" s="21"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
@@ -15624,8 +18514,8 @@
     <row r="5" spans="2:29" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="30"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="225"/>
-      <c r="F5" s="225"/>
+      <c r="E5" s="231"/>
+      <c r="F5" s="231"/>
       <c r="G5" s="17" t="s">
         <v>16</v>
       </c>
@@ -15663,10 +18553,10 @@
     </row>
     <row r="7" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C7" s="87"/>
-      <c r="D7" s="235" t="s">
+      <c r="D7" s="241" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="235"/>
+      <c r="E7" s="241"/>
       <c r="F7" s="178" t="s">
         <v>41</v>
       </c>
@@ -15684,10 +18574,10 @@
       </c>
       <c r="K7" s="160"/>
       <c r="L7" s="161"/>
-      <c r="M7" s="233"/>
-      <c r="N7" s="233"/>
-      <c r="O7" s="233"/>
-      <c r="P7" s="233"/>
+      <c r="M7" s="239"/>
+      <c r="N7" s="239"/>
+      <c r="O7" s="239"/>
+      <c r="P7" s="239"/>
       <c r="Q7" s="88"/>
       <c r="R7" s="89"/>
       <c r="S7" s="34"/>
@@ -15721,10 +18611,10 @@
     </row>
     <row r="9" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C9" s="98"/>
-      <c r="D9" s="236" t="s">
+      <c r="D9" s="242" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="236"/>
+      <c r="E9" s="242"/>
       <c r="F9" s="180" t="s">
         <v>42</v>
       </c>
@@ -15738,10 +18628,10 @@
       <c r="J9" s="165"/>
       <c r="K9" s="165"/>
       <c r="L9" s="165"/>
-      <c r="M9" s="234"/>
-      <c r="N9" s="234"/>
-      <c r="O9" s="234"/>
-      <c r="P9" s="234"/>
+      <c r="M9" s="240"/>
+      <c r="N9" s="240"/>
+      <c r="O9" s="240"/>
+      <c r="P9" s="240"/>
       <c r="Q9" s="99"/>
       <c r="R9" s="90"/>
       <c r="S9" s="100"/>
@@ -15787,10 +18677,10 @@
     </row>
     <row r="11" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="110"/>
-      <c r="D11" s="237" t="s">
+      <c r="D11" s="243" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="237"/>
+      <c r="E11" s="243"/>
       <c r="F11" s="181" t="s">
         <v>43</v>
       </c>
@@ -15806,10 +18696,10 @@
       <c r="J11" s="168"/>
       <c r="K11" s="168"/>
       <c r="L11" s="168"/>
-      <c r="M11" s="240"/>
-      <c r="N11" s="240"/>
-      <c r="O11" s="240"/>
-      <c r="P11" s="240"/>
+      <c r="M11" s="221"/>
+      <c r="N11" s="221"/>
+      <c r="O11" s="221"/>
+      <c r="P11" s="221"/>
       <c r="Q11" s="111"/>
       <c r="R11" s="91"/>
       <c r="S11" s="112"/>
@@ -15855,10 +18745,10 @@
     </row>
     <row r="13" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="122"/>
-      <c r="D13" s="238" t="s">
+      <c r="D13" s="244" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="238"/>
+      <c r="E13" s="244"/>
       <c r="F13" s="182" t="s">
         <v>44</v>
       </c>
@@ -15876,10 +18766,10 @@
       </c>
       <c r="K13" s="171"/>
       <c r="L13" s="171"/>
-      <c r="M13" s="239"/>
-      <c r="N13" s="239"/>
-      <c r="O13" s="239"/>
-      <c r="P13" s="239"/>
+      <c r="M13" s="220"/>
+      <c r="N13" s="220"/>
+      <c r="O13" s="220"/>
+      <c r="P13" s="220"/>
       <c r="Q13" s="123"/>
       <c r="R13" s="93"/>
       <c r="S13" s="124"/>
@@ -15925,10 +18815,10 @@
     </row>
     <row r="15" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="133"/>
-      <c r="D15" s="242" t="s">
+      <c r="D15" s="223" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="242"/>
+      <c r="E15" s="223"/>
       <c r="F15" s="183" t="s">
         <v>45</v>
       </c>
@@ -15948,10 +18838,10 @@
         <v>-20</v>
       </c>
       <c r="L15" s="174"/>
-      <c r="M15" s="241"/>
-      <c r="N15" s="241"/>
-      <c r="O15" s="241"/>
-      <c r="P15" s="241"/>
+      <c r="M15" s="222"/>
+      <c r="N15" s="222"/>
+      <c r="O15" s="222"/>
+      <c r="P15" s="222"/>
       <c r="Q15" s="135"/>
       <c r="R15" s="94"/>
       <c r="S15" s="136"/>
@@ -15997,10 +18887,10 @@
     </row>
     <row r="17" spans="2:29" s="11" customFormat="1" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="143"/>
-      <c r="D17" s="244" t="s">
+      <c r="D17" s="225" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="244"/>
+      <c r="E17" s="225"/>
       <c r="F17" s="184" t="s">
         <v>46</v>
       </c>
@@ -16018,10 +18908,10 @@
       </c>
       <c r="K17" s="177"/>
       <c r="L17" s="177"/>
-      <c r="M17" s="243"/>
-      <c r="N17" s="243"/>
-      <c r="O17" s="243"/>
-      <c r="P17" s="243"/>
+      <c r="M17" s="224"/>
+      <c r="N17" s="224"/>
+      <c r="O17" s="224"/>
+      <c r="P17" s="224"/>
       <c r="Q17" s="145"/>
       <c r="R17" s="90"/>
       <c r="S17" s="144"/>
@@ -16060,22 +18950,22 @@
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
-      <c r="E20" s="224" t="s">
+      <c r="E20" s="230" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="228"/>
-      <c r="G20" s="231" t="s">
+      <c r="F20" s="234"/>
+      <c r="G20" s="237" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220" t="s">
+      <c r="H20" s="226"/>
+      <c r="I20" s="226" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="220"/>
-      <c r="K20" s="220" t="s">
+      <c r="J20" s="226"/>
+      <c r="K20" s="226" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="221"/>
+      <c r="L20" s="227"/>
       <c r="M20" s="44"/>
       <c r="N20" s="45"/>
       <c r="O20" s="45"/>
@@ -16092,21 +18982,21 @@
       <c r="B21" s="28"/>
       <c r="C21" s="28"/>
       <c r="D21" s="28"/>
-      <c r="E21" s="229"/>
-      <c r="F21" s="230"/>
-      <c r="G21" s="232">
+      <c r="E21" s="235"/>
+      <c r="F21" s="236"/>
+      <c r="G21" s="238">
         <v>-10</v>
       </c>
-      <c r="H21" s="232"/>
-      <c r="I21" s="232">
+      <c r="H21" s="238"/>
+      <c r="I21" s="238">
         <v>0.2</v>
       </c>
-      <c r="J21" s="232"/>
-      <c r="K21" s="222">
+      <c r="J21" s="238"/>
+      <c r="K21" s="228">
         <f>G21+100*I21</f>
         <v>10</v>
       </c>
-      <c r="L21" s="222"/>
+      <c r="L21" s="228"/>
       <c r="M21" s="47"/>
       <c r="N21" s="48"/>
       <c r="O21" s="48"/>
@@ -20477,12 +23367,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="9NOS8jY5Ug7YrOY49rx7A6/cXCpIjF5Enxg4kw2PLmKKvG06duBf92zLgkT/MBeWCI1tXrFRs+R4hrI9dhXplw==" saltValue="nRjJWJch2cTa6A5Bi+wDuA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="22">
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="B2:AB2"/>
@@ -20499,6 +23383,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20537,59 +23427,59 @@
     <row r="1" spans="1:28" ht="7" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:28" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="200"/>
-      <c r="B2" s="252" t="s">
+      <c r="B2" s="247" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="252"/>
-      <c r="D2" s="252"/>
-      <c r="E2" s="252"/>
-      <c r="F2" s="252"/>
-      <c r="G2" s="252"/>
-      <c r="H2" s="252"/>
-      <c r="I2" s="252"/>
-      <c r="J2" s="252"/>
-      <c r="K2" s="252"/>
-      <c r="L2" s="252"/>
-      <c r="M2" s="252"/>
-      <c r="N2" s="252"/>
-      <c r="O2" s="252"/>
-      <c r="P2" s="252"/>
-      <c r="Q2" s="252"/>
-      <c r="R2" s="252"/>
-      <c r="S2" s="252"/>
-      <c r="T2" s="252"/>
-      <c r="U2" s="252"/>
-      <c r="V2" s="252"/>
-      <c r="W2" s="252"/>
-      <c r="X2" s="252"/>
-      <c r="Y2" s="252"/>
-      <c r="Z2" s="252"/>
-      <c r="AA2" s="252"/>
-      <c r="AB2" s="252"/>
+      <c r="C2" s="247"/>
+      <c r="D2" s="247"/>
+      <c r="E2" s="247"/>
+      <c r="F2" s="247"/>
+      <c r="G2" s="247"/>
+      <c r="H2" s="247"/>
+      <c r="I2" s="247"/>
+      <c r="J2" s="247"/>
+      <c r="K2" s="247"/>
+      <c r="L2" s="247"/>
+      <c r="M2" s="247"/>
+      <c r="N2" s="247"/>
+      <c r="O2" s="247"/>
+      <c r="P2" s="247"/>
+      <c r="Q2" s="247"/>
+      <c r="R2" s="247"/>
+      <c r="S2" s="247"/>
+      <c r="T2" s="247"/>
+      <c r="U2" s="247"/>
+      <c r="V2" s="247"/>
+      <c r="W2" s="247"/>
+      <c r="X2" s="247"/>
+      <c r="Y2" s="247"/>
+      <c r="Z2" s="247"/>
+      <c r="AA2" s="247"/>
+      <c r="AB2" s="247"/>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="B4" s="250" t="s">
+      <c r="B4" s="245" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="250"/>
-      <c r="D4" s="250"/>
-      <c r="E4" s="250"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="251" t="s">
+      <c r="C4" s="245"/>
+      <c r="D4" s="245"/>
+      <c r="E4" s="245"/>
+      <c r="F4" s="245"/>
+      <c r="G4" s="246" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="251"/>
+      <c r="H4" s="246"/>
+      <c r="I4" s="246"/>
+      <c r="J4" s="246"/>
+      <c r="K4" s="246"/>
+      <c r="L4" s="246"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
+      <c r="B5" s="245"/>
+      <c r="C5" s="245"/>
+      <c r="D5" s="245"/>
+      <c r="E5" s="245"/>
+      <c r="F5" s="245"/>
       <c r="G5" s="202" t="s">
         <v>16</v>
       </c>
@@ -20805,18 +23695,18 @@
       <c r="D20" s="249"/>
       <c r="E20" s="249"/>
       <c r="F20" s="249"/>
-      <c r="G20" s="245" t="s">
+      <c r="G20" s="250" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="245"/>
-      <c r="I20" s="245" t="s">
+      <c r="H20" s="250"/>
+      <c r="I20" s="250" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="245"/>
-      <c r="K20" s="245" t="s">
+      <c r="J20" s="250"/>
+      <c r="K20" s="250" t="s">
         <v>36</v>
       </c>
-      <c r="L20" s="245"/>
+      <c r="L20" s="250"/>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.35">
       <c r="B21" s="249"/>
@@ -20824,18 +23714,18 @@
       <c r="D21" s="249"/>
       <c r="E21" s="249"/>
       <c r="F21" s="249"/>
-      <c r="G21" s="246">
+      <c r="G21" s="251">
         <v>-10</v>
       </c>
-      <c r="H21" s="246"/>
-      <c r="I21" s="246">
+      <c r="H21" s="251"/>
+      <c r="I21" s="251">
         <v>0.2</v>
       </c>
-      <c r="J21" s="246"/>
-      <c r="K21" s="247">
+      <c r="J21" s="251"/>
+      <c r="K21" s="252">
         <v>10</v>
       </c>
-      <c r="L21" s="247"/>
+      <c r="L21" s="252"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.35">
       <c r="B23" s="208"/>
@@ -25144,22 +28034,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:F5"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="B2:AB2"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B20:F21"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="K20:L20"/>
     <mergeCell ref="K21:L21"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B20:F21"/>
+    <mergeCell ref="B4:F5"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="B2:AB2"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25171,7 +28061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:U119"/>
   <sheetViews>
-    <sheetView topLeftCell="E18" workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25197,17 +28087,17 @@
   <sheetData>
     <row r="1" spans="2:21" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="223" t="s">
+      <c r="B2" s="229" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
-      <c r="H2" s="223"/>
-      <c r="I2" s="223"/>
-      <c r="J2" s="223"/>
+      <c r="C2" s="229"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
+      <c r="H2" s="229"/>
+      <c r="I2" s="229"/>
+      <c r="J2" s="229"/>
       <c r="K2" s="70"/>
       <c r="L2" s="70"/>
       <c r="M2" s="70"/>
@@ -25223,16 +28113,16 @@
     <row r="4" spans="2:21" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="29"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="224" t="s">
+      <c r="E4" s="230" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="224"/>
-      <c r="G4" s="226" t="s">
+      <c r="F4" s="230"/>
+      <c r="G4" s="232" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="227"/>
-      <c r="I4" s="227"/>
-      <c r="J4" s="227"/>
+      <c r="H4" s="233"/>
+      <c r="I4" s="233"/>
+      <c r="J4" s="233"/>
       <c r="K4" s="56"/>
       <c r="L4" s="54"/>
       <c r="M4" s="54"/>
@@ -25247,8 +28137,8 @@
     <row r="5" spans="2:21" ht="10.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="30"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="225"/>
-      <c r="F5" s="225"/>
+      <c r="E5" s="231"/>
+      <c r="F5" s="231"/>
       <c r="G5" s="17" t="s">
         <v>16</v>
       </c>
@@ -25466,10 +28356,10 @@
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
-      <c r="E14" s="224" t="s">
+      <c r="E14" s="230" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="228"/>
+      <c r="F14" s="234"/>
       <c r="G14" s="71" t="s">
         <v>24</v>
       </c>
@@ -25495,8 +28385,8 @@
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="E15" s="229"/>
-      <c r="F15" s="230"/>
+      <c r="E15" s="235"/>
+      <c r="F15" s="236"/>
       <c r="G15" s="191">
         <f>-2*PI()</f>
         <v>-6.2831853071795862</v>
@@ -28286,7 +31176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C26ECBF-E433-459E-ADC1-CD84348562CD}">
   <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -28296,7 +31188,9 @@
     <col min="7" max="7" width="15.81640625" style="198" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.453125" style="198"/>
     <col min="9" max="9" width="12.453125" style="198" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.453125" style="198"/>
+    <col min="10" max="13" width="11.453125" style="198"/>
+    <col min="14" max="17" width="0" style="198" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="11.453125" style="198"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.35">
@@ -28313,36 +31207,36 @@
       <c r="J2" s="257"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B4" s="250" t="s">
+      <c r="B4" s="245" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="250"/>
-      <c r="D4" s="250"/>
-      <c r="E4" s="250"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="245" t="s">
+      <c r="C4" s="245"/>
+      <c r="D4" s="245"/>
+      <c r="E4" s="245"/>
+      <c r="F4" s="245"/>
+      <c r="G4" s="250" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="245"/>
-      <c r="I4" s="245"/>
-      <c r="J4" s="245"/>
+      <c r="H4" s="250"/>
+      <c r="I4" s="250"/>
+      <c r="J4" s="250"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B5" s="250"/>
-      <c r="C5" s="250"/>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="206" t="s">
+      <c r="B5" s="245"/>
+      <c r="C5" s="245"/>
+      <c r="D5" s="245"/>
+      <c r="E5" s="245"/>
+      <c r="F5" s="245"/>
+      <c r="G5" s="260" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="206" t="s">
+      <c r="H5" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="206" t="s">
+      <c r="I5" s="261" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="206" t="s">
+      <c r="J5" s="262" t="s">
         <v>19</v>
       </c>
       <c r="O5" s="198" t="s">
@@ -28380,19 +31274,19 @@
       <c r="C7" s="256"/>
       <c r="D7" s="256"/>
       <c r="E7" s="256"/>
-      <c r="F7" s="198" t="s">
+      <c r="F7" s="266" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="218">
+      <c r="G7" s="267">
         <v>2</v>
       </c>
-      <c r="H7" s="218">
+      <c r="H7" s="267">
         <v>2</v>
       </c>
-      <c r="I7" s="218">
+      <c r="I7" s="267">
         <v>0</v>
       </c>
-      <c r="J7" s="218">
+      <c r="J7" s="267">
         <v>0</v>
       </c>
       <c r="N7" s="198">
@@ -28445,19 +31339,19 @@
       <c r="C9" s="256"/>
       <c r="D9" s="256"/>
       <c r="E9" s="256"/>
-      <c r="F9" s="198" t="s">
+      <c r="F9" s="268" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="218">
+      <c r="G9" s="269">
         <v>2</v>
       </c>
-      <c r="H9" s="218">
+      <c r="H9" s="269">
         <v>1</v>
       </c>
-      <c r="I9" s="218">
+      <c r="I9" s="269">
         <v>0</v>
       </c>
-      <c r="J9" s="218">
+      <c r="J9" s="269">
         <v>0</v>
       </c>
       <c r="N9" s="198">
@@ -28506,19 +31400,19 @@
       <c r="C11" s="256"/>
       <c r="D11" s="256"/>
       <c r="E11" s="256"/>
-      <c r="F11" s="198" t="s">
+      <c r="F11" s="270" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="218">
+      <c r="G11" s="271">
         <v>1</v>
       </c>
-      <c r="H11" s="218">
+      <c r="H11" s="271">
         <v>1</v>
       </c>
-      <c r="I11" s="218">
+      <c r="I11" s="271">
         <v>0</v>
       </c>
-      <c r="J11" s="218">
+      <c r="J11" s="271">
         <v>0</v>
       </c>
       <c r="N11" s="198">
@@ -28575,13 +31469,13 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B14" s="251" t="s">
+      <c r="B14" s="246" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="251"/>
-      <c r="D14" s="251"/>
-      <c r="E14" s="251"/>
-      <c r="F14" s="251"/>
+      <c r="C14" s="246"/>
+      <c r="D14" s="246"/>
+      <c r="E14" s="246"/>
+      <c r="F14" s="246"/>
       <c r="G14" s="219" t="s">
         <v>24</v>
       </c>
@@ -28609,18 +31503,18 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B15" s="251"/>
-      <c r="C15" s="251"/>
-      <c r="D15" s="251"/>
-      <c r="E15" s="251"/>
-      <c r="F15" s="251"/>
-      <c r="G15" s="198">
+      <c r="B15" s="246"/>
+      <c r="C15" s="246"/>
+      <c r="D15" s="246"/>
+      <c r="E15" s="246"/>
+      <c r="F15" s="246"/>
+      <c r="G15" s="263">
         <v>-6.2830000000000004</v>
       </c>
-      <c r="H15" s="198">
+      <c r="H15" s="264">
         <v>0.126</v>
       </c>
-      <c r="I15" s="198">
+      <c r="I15" s="265">
         <v>6.2830000000000004</v>
       </c>
       <c r="N15" s="198">
@@ -28658,7 +31552,16 @@
         <v>3.1152516648024537</v>
       </c>
     </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B17" s="208"/>
+      <c r="C17" s="209"/>
+      <c r="D17" s="209"/>
+      <c r="E17" s="209"/>
+      <c r="F17" s="209"/>
+      <c r="G17" s="209"/>
+      <c r="H17" s="209"/>
+      <c r="I17" s="209"/>
+      <c r="J17" s="210"/>
       <c r="N17" s="198">
         <f t="shared" si="3"/>
         <v>-4.8969999999999967</v>
@@ -28676,7 +31579,16 @@
         <v>5.3551174609773442</v>
       </c>
     </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B18" s="211"/>
+      <c r="C18" s="212"/>
+      <c r="D18" s="212"/>
+      <c r="E18" s="212"/>
+      <c r="F18" s="212"/>
+      <c r="G18" s="212"/>
+      <c r="H18" s="212"/>
+      <c r="I18" s="212"/>
+      <c r="J18" s="213"/>
       <c r="N18" s="198">
         <f t="shared" si="3"/>
         <v>-4.7709999999999964</v>
@@ -28694,7 +31606,16 @@
         <v>17.042096526443199</v>
       </c>
     </row>
-    <row r="19" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B19" s="211"/>
+      <c r="C19" s="212"/>
+      <c r="D19" s="212"/>
+      <c r="E19" s="212"/>
+      <c r="F19" s="212"/>
+      <c r="G19" s="212"/>
+      <c r="H19" s="212"/>
+      <c r="I19" s="212"/>
+      <c r="J19" s="213"/>
       <c r="N19" s="198">
         <f t="shared" si="3"/>
         <v>-4.644999999999996</v>
@@ -28712,7 +31633,16 @@
         <v>-14.816751605132295</v>
       </c>
     </row>
-    <row r="20" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B20" s="211"/>
+      <c r="C20" s="212"/>
+      <c r="D20" s="212"/>
+      <c r="E20" s="212"/>
+      <c r="F20" s="212"/>
+      <c r="G20" s="212"/>
+      <c r="H20" s="212"/>
+      <c r="I20" s="212"/>
+      <c r="J20" s="213"/>
       <c r="N20" s="198">
         <f t="shared" si="3"/>
         <v>-4.5189999999999957</v>
@@ -28730,7 +31660,16 @@
         <v>-5.106301155025827</v>
       </c>
     </row>
-    <row r="21" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B21" s="211"/>
+      <c r="C21" s="212"/>
+      <c r="D21" s="212"/>
+      <c r="E21" s="212"/>
+      <c r="F21" s="212"/>
+      <c r="G21" s="212"/>
+      <c r="H21" s="212"/>
+      <c r="I21" s="212"/>
+      <c r="J21" s="213"/>
       <c r="N21" s="198">
         <f t="shared" si="3"/>
         <v>-4.3929999999999954</v>
@@ -28748,7 +31687,16 @@
         <v>-3.0237842894140581</v>
       </c>
     </row>
-    <row r="22" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B22" s="211"/>
+      <c r="C22" s="212"/>
+      <c r="D22" s="212"/>
+      <c r="E22" s="212"/>
+      <c r="F22" s="212"/>
+      <c r="G22" s="212"/>
+      <c r="H22" s="212"/>
+      <c r="I22" s="212"/>
+      <c r="J22" s="213"/>
       <c r="N22" s="198">
         <f t="shared" si="3"/>
         <v>-4.266999999999995</v>
@@ -28766,7 +31714,16 @@
         <v>-2.0947642028376494</v>
       </c>
     </row>
-    <row r="23" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B23" s="211"/>
+      <c r="C23" s="212"/>
+      <c r="D23" s="212"/>
+      <c r="E23" s="212"/>
+      <c r="F23" s="212"/>
+      <c r="G23" s="212"/>
+      <c r="H23" s="212"/>
+      <c r="I23" s="212"/>
+      <c r="J23" s="213"/>
       <c r="N23" s="198">
         <f t="shared" si="3"/>
         <v>-4.1409999999999947</v>
@@ -28784,7 +31741,16 @@
         <v>-1.5553794504950544</v>
       </c>
     </row>
-    <row r="24" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B24" s="211"/>
+      <c r="C24" s="212"/>
+      <c r="D24" s="212"/>
+      <c r="E24" s="212"/>
+      <c r="F24" s="212"/>
+      <c r="G24" s="212"/>
+      <c r="H24" s="212"/>
+      <c r="I24" s="212"/>
+      <c r="J24" s="213"/>
       <c r="N24" s="198">
         <f t="shared" si="3"/>
         <v>-4.0149999999999944</v>
@@ -28802,7 +31768,16 @@
         <v>-1.193552774307163</v>
       </c>
     </row>
-    <row r="25" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B25" s="211"/>
+      <c r="C25" s="212"/>
+      <c r="D25" s="212"/>
+      <c r="E25" s="212"/>
+      <c r="F25" s="212"/>
+      <c r="G25" s="212"/>
+      <c r="H25" s="212"/>
+      <c r="I25" s="212"/>
+      <c r="J25" s="213"/>
       <c r="N25" s="198">
         <f t="shared" si="3"/>
         <v>-3.8889999999999945</v>
@@ -28820,7 +31795,16 @@
         <v>-0.9267653727245575</v>
       </c>
     </row>
-    <row r="26" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B26" s="211"/>
+      <c r="C26" s="212"/>
+      <c r="D26" s="212"/>
+      <c r="E26" s="212"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="212"/>
+      <c r="H26" s="212"/>
+      <c r="I26" s="212"/>
+      <c r="J26" s="213"/>
       <c r="N26" s="198">
         <f t="shared" si="3"/>
         <v>-3.7629999999999946</v>
@@ -28838,7 +31822,16 @@
         <v>-0.71603576798111146</v>
       </c>
     </row>
-    <row r="27" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B27" s="211"/>
+      <c r="C27" s="212"/>
+      <c r="D27" s="212"/>
+      <c r="E27" s="212"/>
+      <c r="F27" s="212"/>
+      <c r="G27" s="212"/>
+      <c r="H27" s="212"/>
+      <c r="I27" s="212"/>
+      <c r="J27" s="213"/>
       <c r="N27" s="198">
         <f t="shared" si="3"/>
         <v>-3.6369999999999947</v>
@@ -28856,7 +31849,16 @@
         <v>-0.54035405793876157</v>
       </c>
     </row>
-    <row r="28" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B28" s="211"/>
+      <c r="C28" s="212"/>
+      <c r="D28" s="212"/>
+      <c r="E28" s="212"/>
+      <c r="F28" s="212"/>
+      <c r="G28" s="212"/>
+      <c r="H28" s="212"/>
+      <c r="I28" s="212"/>
+      <c r="J28" s="213"/>
       <c r="N28" s="198">
         <f t="shared" si="3"/>
         <v>-3.5109999999999948</v>
@@ -28874,7 +31876,16 @@
         <v>-0.38718150715586014</v>
       </c>
     </row>
-    <row r="29" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B29" s="211"/>
+      <c r="C29" s="212"/>
+      <c r="D29" s="212"/>
+      <c r="E29" s="212"/>
+      <c r="F29" s="212"/>
+      <c r="G29" s="212"/>
+      <c r="H29" s="212"/>
+      <c r="I29" s="212"/>
+      <c r="J29" s="213"/>
       <c r="N29" s="198">
         <f t="shared" si="3"/>
         <v>-3.3849999999999949</v>
@@ -28892,7 +31903,16 @@
         <v>-0.24833113019580119</v>
       </c>
     </row>
-    <row r="30" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B30" s="211"/>
+      <c r="C30" s="212"/>
+      <c r="D30" s="212"/>
+      <c r="E30" s="212"/>
+      <c r="F30" s="212"/>
+      <c r="G30" s="212"/>
+      <c r="H30" s="212"/>
+      <c r="I30" s="212"/>
+      <c r="J30" s="213"/>
       <c r="N30" s="198">
         <f t="shared" si="3"/>
         <v>-3.258999999999995</v>
@@ -28910,7 +31930,16 @@
         <v>-0.1179498042086834</v>
       </c>
     </row>
-    <row r="31" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B31" s="211"/>
+      <c r="C31" s="212"/>
+      <c r="D31" s="212"/>
+      <c r="E31" s="212"/>
+      <c r="F31" s="212"/>
+      <c r="G31" s="212"/>
+      <c r="H31" s="212"/>
+      <c r="I31" s="212"/>
+      <c r="J31" s="213"/>
       <c r="N31" s="198">
         <f t="shared" si="3"/>
         <v>-3.1329999999999951</v>
@@ -28928,7 +31957,16 @@
         <v>8.5928650718340941E-3</v>
       </c>
     </row>
-    <row r="32" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B32" s="211"/>
+      <c r="C32" s="212"/>
+      <c r="D32" s="212"/>
+      <c r="E32" s="212"/>
+      <c r="F32" s="212"/>
+      <c r="G32" s="212"/>
+      <c r="H32" s="212"/>
+      <c r="I32" s="212"/>
+      <c r="J32" s="213"/>
       <c r="N32" s="198">
         <f t="shared" si="3"/>
         <v>-3.0069999999999952</v>
@@ -28946,7 +31984,16 @@
         <v>0.13541130963318615</v>
       </c>
     </row>
-    <row r="33" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B33" s="211"/>
+      <c r="C33" s="212"/>
+      <c r="D33" s="212"/>
+      <c r="E33" s="212"/>
+      <c r="F33" s="212"/>
+      <c r="G33" s="212"/>
+      <c r="H33" s="212"/>
+      <c r="I33" s="212"/>
+      <c r="J33" s="213"/>
       <c r="N33" s="198">
         <f t="shared" si="3"/>
         <v>-2.8809999999999953</v>
@@ -28964,7 +32011,16 @@
         <v>0.26665623604500688</v>
       </c>
     </row>
-    <row r="34" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B34" s="211"/>
+      <c r="C34" s="212"/>
+      <c r="D34" s="212"/>
+      <c r="E34" s="212"/>
+      <c r="F34" s="212"/>
+      <c r="G34" s="212"/>
+      <c r="H34" s="212"/>
+      <c r="I34" s="212"/>
+      <c r="J34" s="213"/>
       <c r="N34" s="198">
         <f t="shared" si="3"/>
         <v>-2.7549999999999955</v>
@@ -28982,7 +32038,16 @@
         <v>0.40707739810346705</v>
       </c>
     </row>
-    <row r="35" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B35" s="211"/>
+      <c r="C35" s="212"/>
+      <c r="D35" s="212"/>
+      <c r="E35" s="212"/>
+      <c r="F35" s="212"/>
+      <c r="G35" s="212"/>
+      <c r="H35" s="212"/>
+      <c r="I35" s="212"/>
+      <c r="J35" s="213"/>
       <c r="N35" s="198">
         <f t="shared" si="3"/>
         <v>-2.6289999999999956</v>
@@ -29000,7 +32065,16 @@
         <v>0.5627675154822025</v>
       </c>
     </row>
-    <row r="36" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B36" s="211"/>
+      <c r="C36" s="212"/>
+      <c r="D36" s="212"/>
+      <c r="E36" s="212"/>
+      <c r="F36" s="212"/>
+      <c r="G36" s="212"/>
+      <c r="H36" s="212"/>
+      <c r="I36" s="212"/>
+      <c r="J36" s="213"/>
       <c r="N36" s="198">
         <f t="shared" si="3"/>
         <v>-2.5029999999999957</v>
@@ -29018,7 +32092,16 @@
         <v>0.74235860794953468</v>
       </c>
     </row>
-    <row r="37" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B37" s="211"/>
+      <c r="C37" s="212"/>
+      <c r="D37" s="212"/>
+      <c r="E37" s="212"/>
+      <c r="F37" s="212"/>
+      <c r="G37" s="212"/>
+      <c r="H37" s="212"/>
+      <c r="I37" s="212"/>
+      <c r="J37" s="213"/>
       <c r="N37" s="198">
         <f t="shared" si="3"/>
         <v>-2.3769999999999958</v>
@@ -29036,7 +32119,16 @@
         <v>0.95923131106856674</v>
       </c>
     </row>
-    <row r="38" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B38" s="211"/>
+      <c r="C38" s="212"/>
+      <c r="D38" s="212"/>
+      <c r="E38" s="212"/>
+      <c r="F38" s="212"/>
+      <c r="G38" s="212"/>
+      <c r="H38" s="212"/>
+      <c r="I38" s="212"/>
+      <c r="J38" s="213"/>
       <c r="N38" s="198">
         <f t="shared" si="3"/>
         <v>-2.2509999999999959</v>
@@ -29054,7 +32146,16 @@
         <v>1.2360965520547245</v>
       </c>
     </row>
-    <row r="39" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B39" s="211"/>
+      <c r="C39" s="212"/>
+      <c r="D39" s="212"/>
+      <c r="E39" s="212"/>
+      <c r="F39" s="212"/>
+      <c r="G39" s="212"/>
+      <c r="H39" s="212"/>
+      <c r="I39" s="212"/>
+      <c r="J39" s="213"/>
       <c r="N39" s="198">
         <f t="shared" si="3"/>
         <v>-2.124999999999996</v>
@@ -29072,7 +32173,16 @@
         <v>1.6157594239734745</v>
       </c>
     </row>
-    <row r="40" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B40" s="211"/>
+      <c r="C40" s="212"/>
+      <c r="D40" s="212"/>
+      <c r="E40" s="212"/>
+      <c r="F40" s="212"/>
+      <c r="G40" s="212"/>
+      <c r="H40" s="212"/>
+      <c r="I40" s="212"/>
+      <c r="J40" s="213"/>
       <c r="N40" s="198">
         <f t="shared" si="3"/>
         <v>-1.9989999999999961</v>
@@ -29090,7 +32200,16 @@
         <v>2.1908269093209292</v>
       </c>
     </row>
-    <row r="41" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B41" s="211"/>
+      <c r="C41" s="212"/>
+      <c r="D41" s="212"/>
+      <c r="E41" s="212"/>
+      <c r="F41" s="212"/>
+      <c r="G41" s="212"/>
+      <c r="H41" s="212"/>
+      <c r="I41" s="212"/>
+      <c r="J41" s="213"/>
       <c r="N41" s="198">
         <f t="shared" si="3"/>
         <v>-1.8729999999999962</v>
@@ -29108,7 +32227,16 @@
         <v>3.2076733614779225</v>
       </c>
     </row>
-    <row r="42" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B42" s="211"/>
+      <c r="C42" s="212"/>
+      <c r="D42" s="212"/>
+      <c r="E42" s="212"/>
+      <c r="F42" s="212"/>
+      <c r="G42" s="212"/>
+      <c r="H42" s="212"/>
+      <c r="I42" s="212"/>
+      <c r="J42" s="213"/>
       <c r="N42" s="198">
         <f t="shared" si="3"/>
         <v>-1.7469999999999963</v>
@@ -29126,7 +32254,16 @@
         <v>5.6163940982019902</v>
       </c>
     </row>
-    <row r="43" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B43" s="211"/>
+      <c r="C43" s="212"/>
+      <c r="D43" s="212"/>
+      <c r="E43" s="212"/>
+      <c r="F43" s="212"/>
+      <c r="G43" s="212"/>
+      <c r="H43" s="212"/>
+      <c r="I43" s="212"/>
+      <c r="J43" s="213"/>
       <c r="N43" s="198">
         <f t="shared" si="3"/>
         <v>-1.6209999999999964</v>
@@ -29144,7 +32281,16 @@
         <v>19.902123863539483</v>
       </c>
     </row>
-    <row r="44" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B44" s="211"/>
+      <c r="C44" s="212"/>
+      <c r="D44" s="212"/>
+      <c r="E44" s="212"/>
+      <c r="F44" s="212"/>
+      <c r="G44" s="212"/>
+      <c r="H44" s="212"/>
+      <c r="I44" s="212"/>
+      <c r="J44" s="213"/>
       <c r="N44" s="198">
         <f t="shared" si="3"/>
         <v>-1.4949999999999966</v>
@@ -29162,7 +32308,16 @@
         <v>-13.167976346854354</v>
       </c>
     </row>
-    <row r="45" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B45" s="211"/>
+      <c r="C45" s="212"/>
+      <c r="D45" s="212"/>
+      <c r="E45" s="212"/>
+      <c r="F45" s="212"/>
+      <c r="G45" s="212"/>
+      <c r="H45" s="212"/>
+      <c r="I45" s="212"/>
+      <c r="J45" s="213"/>
       <c r="N45" s="198">
         <f t="shared" si="3"/>
         <v>-1.3689999999999967</v>
@@ -29180,7 +32335,16 @@
         <v>-4.8880428238793456</v>
       </c>
     </row>
-    <row r="46" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B46" s="211"/>
+      <c r="C46" s="212"/>
+      <c r="D46" s="212"/>
+      <c r="E46" s="212"/>
+      <c r="F46" s="212"/>
+      <c r="G46" s="212"/>
+      <c r="H46" s="212"/>
+      <c r="I46" s="212"/>
+      <c r="J46" s="213"/>
       <c r="N46" s="198">
         <f t="shared" si="3"/>
         <v>-1.2429999999999968</v>
@@ -29198,7 +32362,16 @@
         <v>-2.9406185723143499</v>
       </c>
     </row>
-    <row r="47" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B47" s="214"/>
+      <c r="C47" s="215"/>
+      <c r="D47" s="215"/>
+      <c r="E47" s="215"/>
+      <c r="F47" s="215"/>
+      <c r="G47" s="215"/>
+      <c r="H47" s="215"/>
+      <c r="I47" s="215"/>
+      <c r="J47" s="216"/>
       <c r="N47" s="198">
         <f t="shared" si="3"/>
         <v>-1.1169999999999969</v>
@@ -29216,7 +32389,7 @@
         <v>-2.0502480520082926</v>
       </c>
     </row>
-    <row r="48" spans="14:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.35">
       <c r="N48" s="198">
         <f t="shared" si="3"/>
         <v>-0.99099999999999688</v>
@@ -29650,7 +32823,7 @@
     </row>
     <row r="72" spans="14:17" x14ac:dyDescent="0.35">
       <c r="N72" s="198">
-        <f t="shared" ref="N72:N107" si="7">N71 + $H$15</f>
+        <f t="shared" ref="N72:N106" si="7">N71 + $H$15</f>
         <v>2.0330000000000021</v>
       </c>
       <c r="O72" s="198">
@@ -30290,6 +33463,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>